<commit_message>
agegando colores a las celdas
</commit_message>
<xml_diff>
--- a/assets/Mangas.xlsx
+++ b/assets/Mangas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahue\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9547FF0D-C90F-4957-851E-FE958B4AFF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F4FD8F-7C4D-4ADD-B609-7694F7E3D0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6765F00-11DB-40F5-BC3F-F1F6DA2C76AC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="248">
   <si>
     <t>Tomos</t>
   </si>
@@ -355,9 +355,6 @@
   </si>
   <si>
     <t>Sacerdotisa de la Oscuridad - 2</t>
-  </si>
-  <si>
-    <t>ivrea</t>
   </si>
   <si>
     <t>Goodbye Eri</t>
@@ -1927,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD5DF50-6FBC-4F7F-9AF4-AF00221DFCCC}">
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,10 +1970,10 @@
         <v>6</v>
       </c>
       <c r="I1" s="81" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J1" s="81" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K1" s="81" t="s">
         <v>104</v>
@@ -2009,13 +2006,13 @@
         <v>7</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K2" s="73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2045,13 +2042,13 @@
         <v>7</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K3" s="74" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2081,13 +2078,13 @@
         <v>7</v>
       </c>
       <c r="I4" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K4" s="73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2117,13 +2114,13 @@
         <v>7</v>
       </c>
       <c r="I5" s="51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J5" s="51" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K5" s="73" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2153,10 +2150,10 @@
         <v>7</v>
       </c>
       <c r="I6" s="51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J6" s="51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K6" s="73" t="s">
         <v>105</v>
@@ -2189,10 +2186,10 @@
         <v>7</v>
       </c>
       <c r="I7" s="51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2222,10 +2219,10 @@
         <v>11</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J8" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2255,13 +2252,13 @@
         <v>7</v>
       </c>
       <c r="I9" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K9" s="73" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2291,13 +2288,13 @@
         <v>7</v>
       </c>
       <c r="I10" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J10" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K10" s="73" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2327,10 +2324,10 @@
         <v>7</v>
       </c>
       <c r="I11" s="51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J11" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2360,13 +2357,13 @@
         <v>7</v>
       </c>
       <c r="I12" s="51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J12" s="51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K12" s="73" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2396,13 +2393,13 @@
         <v>12</v>
       </c>
       <c r="I13" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J13" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K13" s="73" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2413,7 +2410,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D14" s="48">
         <v>2</v>
@@ -2432,13 +2429,13 @@
         <v>3</v>
       </c>
       <c r="I14" s="51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J14" s="51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K14" s="73" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2468,13 +2465,13 @@
         <v>7</v>
       </c>
       <c r="I15" s="51" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J15" s="51" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K15" s="73" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2504,13 +2501,13 @@
         <v>7</v>
       </c>
       <c r="I16" s="51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J16" s="51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K16" s="73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2540,10 +2537,10 @@
         <v>7</v>
       </c>
       <c r="I17" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J17" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2573,13 +2570,13 @@
         <v>7</v>
       </c>
       <c r="I18" s="51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J18" s="51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K18" s="73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2609,13 +2606,13 @@
         <v>11</v>
       </c>
       <c r="I19" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J19" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K19" s="73" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2645,13 +2642,13 @@
         <v>7</v>
       </c>
       <c r="I20" s="51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J20" s="51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K20" s="73" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2681,13 +2678,13 @@
         <v>7</v>
       </c>
       <c r="I21" s="51" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J21" s="51" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K21" s="73" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2717,13 +2714,13 @@
         <v>7</v>
       </c>
       <c r="I22" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="J22" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="J22" s="51" t="s">
-        <v>148</v>
-      </c>
       <c r="K22" s="73" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2753,10 +2750,10 @@
         <v>7</v>
       </c>
       <c r="I23" s="51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J23" s="51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2767,7 +2764,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D24" s="48">
         <v>4</v>
@@ -2786,13 +2783,13 @@
         <v>7</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J24" s="51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K24" s="73" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2800,10 +2797,10 @@
         <v>38</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D25" s="48">
         <v>1</v>
@@ -2822,13 +2819,13 @@
         <v>3</v>
       </c>
       <c r="I25" s="51" t="s">
+        <v>243</v>
+      </c>
+      <c r="J25" s="51" t="s">
+        <v>243</v>
+      </c>
+      <c r="K25" s="73" t="s">
         <v>244</v>
-      </c>
-      <c r="J25" s="51" t="s">
-        <v>244</v>
-      </c>
-      <c r="K25" s="73" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2836,10 +2833,10 @@
         <v>38</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D26" s="48">
         <v>1</v>
@@ -2858,13 +2855,13 @@
         <v>3</v>
       </c>
       <c r="I26" s="51" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J26" s="51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K26" s="73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2894,13 +2891,13 @@
         <v>28</v>
       </c>
       <c r="I27" s="51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J27" s="51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K27" s="72" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2911,7 +2908,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D28" s="35">
         <v>2</v>
@@ -2930,10 +2927,10 @@
         <v>2</v>
       </c>
       <c r="I28" s="75" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J28" s="75" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2944,7 +2941,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D29" s="48">
         <v>2</v>
@@ -2963,13 +2960,13 @@
         <v>2</v>
       </c>
       <c r="I29" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="J29" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="J29" s="51" t="s">
+      <c r="K29" s="73" t="s">
         <v>211</v>
-      </c>
-      <c r="K29" s="73" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2996,13 +2993,13 @@
         <v>126500</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I30" s="51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J30" s="51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3032,10 +3029,10 @@
         <v>53</v>
       </c>
       <c r="I31" s="51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J31" s="51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3065,13 +3062,13 @@
         <v>8</v>
       </c>
       <c r="I32" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J32" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K32" s="73" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3101,13 +3098,13 @@
         <v>2</v>
       </c>
       <c r="I33" s="51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J33" s="51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K33" s="73" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3137,10 +3134,10 @@
         <v>3</v>
       </c>
       <c r="I34" s="51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J34" s="51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K34" s="73" t="s">
         <v>106</v>
@@ -3173,10 +3170,10 @@
         <v>13</v>
       </c>
       <c r="I35" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J35" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3206,10 +3203,10 @@
         <v>8</v>
       </c>
       <c r="I36" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J36" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3239,10 +3236,10 @@
         <v>4</v>
       </c>
       <c r="I37" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="J37" s="51" t="s">
         <v>158</v>
-      </c>
-      <c r="J37" s="51" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3272,10 +3269,10 @@
         <v>3</v>
       </c>
       <c r="I38" s="51" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J38" s="51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3305,10 +3302,10 @@
         <v>3</v>
       </c>
       <c r="I39" s="51" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J39" s="51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3338,10 +3335,10 @@
         <v>3</v>
       </c>
       <c r="I40" s="51" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J40" s="51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3371,10 +3368,10 @@
         <v>2</v>
       </c>
       <c r="I41" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="J41" s="51" t="s">
         <v>161</v>
-      </c>
-      <c r="J41" s="51" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3382,10 +3379,10 @@
         <v>39</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D42" s="48">
         <v>4</v>
@@ -3404,13 +3401,13 @@
         <v>4</v>
       </c>
       <c r="I42" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J42" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K42" s="73" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3418,10 +3415,10 @@
         <v>39</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D43" s="48">
         <v>3</v>
@@ -3440,13 +3437,13 @@
         <v>3</v>
       </c>
       <c r="I43" s="51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J43" s="51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K43" s="73" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3476,13 +3473,13 @@
         <v>2</v>
       </c>
       <c r="I44" s="51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J44" s="51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K44" s="73" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3512,10 +3509,10 @@
         <v>3</v>
       </c>
       <c r="I45" s="51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J45" s="51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K45" s="73" t="s">
         <v>107</v>
@@ -3548,13 +3545,13 @@
         <v>5</v>
       </c>
       <c r="I46" s="51" t="s">
+        <v>163</v>
+      </c>
+      <c r="J46" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="J46" s="51" t="s">
-        <v>165</v>
-      </c>
       <c r="K46" s="73" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3584,10 +3581,10 @@
         <v>3</v>
       </c>
       <c r="I47" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J47" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K47" s="73" t="s">
         <v>108</v>
@@ -3620,10 +3617,10 @@
         <v>2</v>
       </c>
       <c r="I48" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J48" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3653,10 +3650,10 @@
         <v>2</v>
       </c>
       <c r="I49" s="51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J49" s="51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K49" s="73" t="s">
         <v>109</v>
@@ -3689,10 +3686,10 @@
         <v>7</v>
       </c>
       <c r="I50" s="51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J50" s="51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3722,10 +3719,10 @@
         <v>9</v>
       </c>
       <c r="I51" s="51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J51" s="51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3755,10 +3752,10 @@
         <v>31</v>
       </c>
       <c r="I52" s="51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J52" s="51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3788,10 +3785,10 @@
         <v>31</v>
       </c>
       <c r="I53" s="51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J53" s="51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3821,10 +3818,10 @@
         <v>23</v>
       </c>
       <c r="I54" s="51" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J54" s="51" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3854,10 +3851,10 @@
         <v>7</v>
       </c>
       <c r="I55" s="51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J55" s="51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3887,10 +3884,10 @@
         <v>7</v>
       </c>
       <c r="I56" s="51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J56" s="51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3920,10 +3917,10 @@
         <v>7</v>
       </c>
       <c r="I57" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J57" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3953,10 +3950,10 @@
         <v>7</v>
       </c>
       <c r="I58" s="51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J58" s="51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3986,10 +3983,10 @@
         <v>7</v>
       </c>
       <c r="I59" s="51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J59" s="51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4019,10 +4016,10 @@
         <v>13</v>
       </c>
       <c r="I60" s="51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J60" s="51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4052,10 +4049,10 @@
         <v>7</v>
       </c>
       <c r="I61" s="51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J61" s="51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4085,10 +4082,10 @@
         <v>1</v>
       </c>
       <c r="I62" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J62" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4118,10 +4115,10 @@
         <v>1</v>
       </c>
       <c r="I63" s="51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J63" s="51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4151,10 +4148,10 @@
         <v>1</v>
       </c>
       <c r="I64" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J64" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4184,10 +4181,10 @@
         <v>1</v>
       </c>
       <c r="I65" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J65" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4217,10 +4214,10 @@
         <v>1</v>
       </c>
       <c r="I66" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J66" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4250,10 +4247,10 @@
         <v>1</v>
       </c>
       <c r="I67" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J67" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4283,10 +4280,10 @@
         <v>1</v>
       </c>
       <c r="I68" s="51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J68" s="51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4316,10 +4313,10 @@
         <v>1</v>
       </c>
       <c r="I69" s="51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J69" s="51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4349,10 +4346,10 @@
         <v>1</v>
       </c>
       <c r="I70" s="51" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J70" s="51" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K70" s="73" t="s">
         <v>85</v>
@@ -4385,10 +4382,10 @@
         <v>1</v>
       </c>
       <c r="I71" s="51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J71" s="51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K71" s="73" t="s">
         <v>86</v>
@@ -4421,10 +4418,10 @@
         <v>1</v>
       </c>
       <c r="I72" s="51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J72" s="51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K72" s="73" t="s">
         <v>87</v>
@@ -4435,10 +4432,10 @@
         <v>64</v>
       </c>
       <c r="B73" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" s="43" t="s">
         <v>110</v>
-      </c>
-      <c r="C73" s="43" t="s">
-        <v>111</v>
       </c>
       <c r="D73" s="44">
         <v>1</v>
@@ -4457,10 +4454,10 @@
         <v>1</v>
       </c>
       <c r="I73" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J73" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4471,7 +4468,7 @@
         <v>24</v>
       </c>
       <c r="C74" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D74" s="35">
         <v>1</v>
@@ -4490,13 +4487,13 @@
         <v>1</v>
       </c>
       <c r="I74" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J74" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K74" s="73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4507,7 +4504,7 @@
         <v>24</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D75" s="48">
         <v>1</v>
@@ -4526,13 +4523,13 @@
         <v>1</v>
       </c>
       <c r="I75" s="51" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J75" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K75" s="73" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4543,7 +4540,7 @@
         <v>24</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D76" s="48">
         <v>1</v>
@@ -4562,13 +4559,13 @@
         <v>1</v>
       </c>
       <c r="I76" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="J76" s="51" t="s">
         <v>202</v>
       </c>
-      <c r="J76" s="51" t="s">
-        <v>203</v>
-      </c>
       <c r="K76" s="73" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4598,10 +4595,10 @@
         <v>1</v>
       </c>
       <c r="I77" s="51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J77" s="51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K77" s="73" t="s">
         <v>67</v>
@@ -4634,10 +4631,10 @@
         <v>1</v>
       </c>
       <c r="I78" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J78" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4667,10 +4664,10 @@
         <v>1</v>
       </c>
       <c r="I79" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J79" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4700,10 +4697,10 @@
         <v>1</v>
       </c>
       <c r="I80" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J80" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4733,10 +4730,10 @@
         <v>1</v>
       </c>
       <c r="I81" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J81" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4747,7 +4744,7 @@
         <v>24</v>
       </c>
       <c r="C82" s="38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D82" s="35">
         <v>1</v>
@@ -4766,10 +4763,10 @@
         <v>1</v>
       </c>
       <c r="I82" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J82" s="75" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4799,10 +4796,10 @@
         <v>1</v>
       </c>
       <c r="I83" s="51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J83" s="51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4832,10 +4829,10 @@
         <v>1</v>
       </c>
       <c r="I84" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J84" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K84" s="73" t="s">
         <v>93</v>
@@ -4868,10 +4865,10 @@
         <v>1</v>
       </c>
       <c r="I85" s="51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J85" s="51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K85" s="73" t="s">
         <v>72</v>
@@ -4904,10 +4901,10 @@
         <v>1</v>
       </c>
       <c r="I86" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J86" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4937,10 +4934,10 @@
         <v>1</v>
       </c>
       <c r="I87" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J87" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4970,10 +4967,10 @@
         <v>1</v>
       </c>
       <c r="I88" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J88" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4984,7 +4981,7 @@
         <v>28</v>
       </c>
       <c r="C89" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D89" s="24">
         <v>1</v>
@@ -5003,13 +5000,13 @@
         <v>1</v>
       </c>
       <c r="I89" s="51" t="s">
+        <v>205</v>
+      </c>
+      <c r="J89" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="J89" s="51" t="s">
-        <v>207</v>
-      </c>
       <c r="K89" s="73" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5039,10 +5036,10 @@
         <v>1</v>
       </c>
       <c r="I90" s="51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J90" s="51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K90" s="73" t="s">
         <v>75</v>
@@ -5056,7 +5053,7 @@
         <v>30</v>
       </c>
       <c r="C91" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D91" s="24">
         <v>1</v>
@@ -5075,13 +5072,13 @@
         <v>1</v>
       </c>
       <c r="I91" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J91" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K91" s="73" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5092,7 +5089,7 @@
         <v>34</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D92" s="48">
         <v>1</v>
@@ -5111,13 +5108,13 @@
         <v>1</v>
       </c>
       <c r="I92" s="51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J92" s="51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K92" s="73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5147,10 +5144,10 @@
         <v>1</v>
       </c>
       <c r="I93" s="51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J93" s="51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5158,10 +5155,10 @@
         <v>64</v>
       </c>
       <c r="B94" s="79" t="s">
+        <v>221</v>
+      </c>
+      <c r="C94" s="31" t="s">
         <v>222</v>
-      </c>
-      <c r="C94" s="31" t="s">
-        <v>223</v>
       </c>
       <c r="D94" s="48">
         <v>1</v>
@@ -5180,13 +5177,13 @@
         <v>1</v>
       </c>
       <c r="I94" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J94" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K94" s="73" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5203,7 +5200,7 @@
         <v>0</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>2</v>
@@ -5212,13 +5209,13 @@
         <v>3</v>
       </c>
       <c r="H95" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I95" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J95" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Terminado todos los estilos
</commit_message>
<xml_diff>
--- a/assets/Mangas.xlsx
+++ b/assets/Mangas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahue\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F4FD8F-7C4D-4ADD-B609-7694F7E3D0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62429EE-83EA-4445-9E1F-088DC8C0C980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6765F00-11DB-40F5-BC3F-F1F6DA2C76AC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="260">
   <si>
     <t>Tomos</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Your Lie in April</t>
   </si>
   <si>
-    <t>11 + 1 OVA</t>
-  </si>
-  <si>
     <t>Darling in the Franxx</t>
   </si>
   <si>
@@ -360,9 +357,6 @@
     <t>Goodbye Eri</t>
   </si>
   <si>
-    <t>20 + 1 OVA</t>
-  </si>
-  <si>
     <t>El Fin del Mundo y Antes del Amanecer</t>
   </si>
   <si>
@@ -769,6 +763,48 @@
   </si>
   <si>
     <t>La Tierra de las Gemas</t>
+  </si>
+  <si>
+    <t>Finalizado (11)</t>
+  </si>
+  <si>
+    <t>Finalizado (12)</t>
+  </si>
+  <si>
+    <t>Finalizado (3)</t>
+  </si>
+  <si>
+    <t>Finalizado (28)</t>
+  </si>
+  <si>
+    <t>Finalizado (2)</t>
+  </si>
+  <si>
+    <t>Finalizado (21)</t>
+  </si>
+  <si>
+    <t>Finalizado (8)</t>
+  </si>
+  <si>
+    <t>Finalizado (13)</t>
+  </si>
+  <si>
+    <t>Finalizado (4)</t>
+  </si>
+  <si>
+    <t>Finalizado (5)</t>
+  </si>
+  <si>
+    <t>Finalizado (9)</t>
+  </si>
+  <si>
+    <t>Finalizado (31)</t>
+  </si>
+  <si>
+    <t>Finalizado (23)</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
   </si>
 </sst>
 </file>
@@ -1924,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD5DF50-6FBC-4F7F-9AF4-AF00221DFCCC}">
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,13 +2006,13 @@
         <v>6</v>
       </c>
       <c r="I1" s="81" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J1" s="81" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K1" s="81" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2006,13 +2042,13 @@
         <v>7</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K2" s="73" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2042,13 +2078,13 @@
         <v>7</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K3" s="74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2078,13 +2114,13 @@
         <v>7</v>
       </c>
       <c r="I4" s="51" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K4" s="73" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2114,13 +2150,13 @@
         <v>7</v>
       </c>
       <c r="I5" s="51" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J5" s="51" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K5" s="73" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2150,13 +2186,13 @@
         <v>7</v>
       </c>
       <c r="I6" s="51" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J6" s="51" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K6" s="73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2186,10 +2222,10 @@
         <v>7</v>
       </c>
       <c r="I7" s="51" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2215,14 +2251,14 @@
         <f t="shared" si="0"/>
         <v>36000</v>
       </c>
-      <c r="H8" s="5">
-        <v>11</v>
+      <c r="H8" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J8" s="51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2233,7 +2269,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="48">
         <v>3</v>
@@ -2252,13 +2288,13 @@
         <v>7</v>
       </c>
       <c r="I9" s="51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K9" s="73" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2269,7 +2305,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" s="48">
         <v>2</v>
@@ -2288,13 +2324,13 @@
         <v>7</v>
       </c>
       <c r="I10" s="51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J10" s="51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K10" s="73" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2324,10 +2360,10 @@
         <v>7</v>
       </c>
       <c r="I11" s="51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J11" s="51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2357,13 +2393,13 @@
         <v>7</v>
       </c>
       <c r="I12" s="51" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J12" s="51" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K12" s="73" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2374,7 +2410,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" s="48">
         <v>5</v>
@@ -2389,17 +2425,17 @@
         <f t="shared" si="0"/>
         <v>27500</v>
       </c>
-      <c r="H13" s="5">
-        <v>12</v>
+      <c r="H13" s="5" t="s">
+        <v>247</v>
       </c>
       <c r="I13" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J13" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K13" s="73" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2410,7 +2446,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D14" s="48">
         <v>2</v>
@@ -2425,17 +2461,17 @@
         <f t="shared" ref="G14:G28" si="1">D14*E14</f>
         <v>13800</v>
       </c>
-      <c r="H14" s="5">
-        <v>3</v>
+      <c r="H14" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I14" s="51" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J14" s="51" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K14" s="73" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2446,7 +2482,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" s="48">
         <v>12</v>
@@ -2465,13 +2501,13 @@
         <v>7</v>
       </c>
       <c r="I15" s="51" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J15" s="51" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K15" s="73" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2482,7 +2518,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D16" s="48">
         <v>18</v>
@@ -2501,13 +2537,13 @@
         <v>7</v>
       </c>
       <c r="I16" s="51" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J16" s="51" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K16" s="73" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2537,10 +2573,10 @@
         <v>7</v>
       </c>
       <c r="I17" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J17" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2570,13 +2606,13 @@
         <v>7</v>
       </c>
       <c r="I18" s="51" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J18" s="51" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K18" s="73" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2602,17 +2638,17 @@
         <f t="shared" si="1"/>
         <v>44000</v>
       </c>
-      <c r="H19" s="5">
-        <v>11</v>
+      <c r="H19" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="I19" s="51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J19" s="51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K19" s="73" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2642,13 +2678,13 @@
         <v>7</v>
       </c>
       <c r="I20" s="51" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J20" s="51" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K20" s="73" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2659,7 +2695,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="48">
         <v>4</v>
@@ -2678,13 +2714,13 @@
         <v>7</v>
       </c>
       <c r="I21" s="51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J21" s="51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K21" s="73" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2714,13 +2750,13 @@
         <v>7</v>
       </c>
       <c r="I22" s="51" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J22" s="51" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K22" s="73" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2750,10 +2786,10 @@
         <v>7</v>
       </c>
       <c r="I23" s="51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J23" s="51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2764,7 +2800,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D24" s="48">
         <v>4</v>
@@ -2783,13 +2819,13 @@
         <v>7</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J24" s="51" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K24" s="73" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2797,10 +2833,10 @@
         <v>38</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D25" s="48">
         <v>1</v>
@@ -2815,17 +2851,17 @@
         <f t="shared" ref="G25" si="2">D25*E25</f>
         <v>9800</v>
       </c>
-      <c r="H25" s="5">
-        <v>3</v>
+      <c r="H25" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I25" s="51" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J25" s="51" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K25" s="73" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2833,10 +2869,10 @@
         <v>38</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D26" s="48">
         <v>1</v>
@@ -2851,17 +2887,17 @@
         <f t="shared" si="1"/>
         <v>12000</v>
       </c>
-      <c r="H26" s="5">
-        <v>3</v>
+      <c r="H26" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I26" s="51" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J26" s="51" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K26" s="73" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2872,7 +2908,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" s="48">
         <v>28</v>
@@ -2887,17 +2923,17 @@
         <f t="shared" si="1"/>
         <v>168000</v>
       </c>
-      <c r="H27" s="5">
-        <v>28</v>
+      <c r="H27" s="5" t="s">
+        <v>249</v>
       </c>
       <c r="I27" s="51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J27" s="51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K27" s="72" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2908,7 +2944,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D28" s="35">
         <v>2</v>
@@ -2923,14 +2959,14 @@
         <f t="shared" si="1"/>
         <v>12000</v>
       </c>
-      <c r="H28" s="37">
-        <v>2</v>
+      <c r="H28" s="37" t="s">
+        <v>250</v>
       </c>
       <c r="I28" s="75" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J28" s="75" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2941,7 +2977,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D29" s="48">
         <v>2</v>
@@ -2956,17 +2992,17 @@
         <f t="shared" ref="G29" si="3">D29*E29</f>
         <v>12000</v>
       </c>
-      <c r="H29" s="5">
-        <v>2</v>
+      <c r="H29" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="I29" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="J29" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="K29" s="73" t="s">
         <v>209</v>
-      </c>
-      <c r="J29" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="K29" s="73" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2993,13 +3029,13 @@
         <v>126500</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>111</v>
+        <v>251</v>
       </c>
       <c r="I30" s="51" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J30" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3026,13 +3062,13 @@
         <v>66000</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>53</v>
+        <v>247</v>
       </c>
       <c r="I31" s="51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J31" s="51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3058,17 +3094,17 @@
         <f>D32*E32</f>
         <v>44000</v>
       </c>
-      <c r="H32" s="5">
-        <v>8</v>
+      <c r="H32" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="I32" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J32" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K32" s="73" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3079,7 +3115,7 @@
         <v>24</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" s="48">
         <v>2</v>
@@ -3094,17 +3130,17 @@
         <f t="shared" si="4"/>
         <v>11000</v>
       </c>
-      <c r="H33" s="5">
-        <v>2</v>
+      <c r="H33" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="I33" s="51" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J33" s="51" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K33" s="73" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3130,17 +3166,17 @@
         <f t="shared" si="4"/>
         <v>16500</v>
       </c>
-      <c r="H34" s="5">
-        <v>3</v>
+      <c r="H34" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I34" s="51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J34" s="51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K34" s="73" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3166,14 +3202,14 @@
         <f t="shared" si="4"/>
         <v>71500</v>
       </c>
-      <c r="H35" s="5">
-        <v>13</v>
+      <c r="H35" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="I35" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J35" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3184,7 +3220,7 @@
         <v>24</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36" s="48">
         <v>8</v>
@@ -3199,14 +3235,14 @@
         <f t="shared" si="4"/>
         <v>44000</v>
       </c>
-      <c r="H36" s="5">
-        <v>8</v>
+      <c r="H36" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="I36" s="51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J36" s="51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3217,7 +3253,7 @@
         <v>24</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="48">
         <v>4</v>
@@ -3232,14 +3268,14 @@
         <f t="shared" si="4"/>
         <v>22000</v>
       </c>
-      <c r="H37" s="5">
-        <v>4</v>
+      <c r="H37" s="5" t="s">
+        <v>254</v>
       </c>
       <c r="I37" s="51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J37" s="51" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3250,7 +3286,7 @@
         <v>24</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D38" s="48">
         <v>3</v>
@@ -3265,14 +3301,14 @@
         <f t="shared" si="4"/>
         <v>16500</v>
       </c>
-      <c r="H38" s="5">
-        <v>3</v>
+      <c r="H38" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I38" s="51" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J38" s="51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3283,7 +3319,7 @@
         <v>24</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D39" s="48">
         <v>3</v>
@@ -3298,14 +3334,14 @@
         <f t="shared" si="4"/>
         <v>16500</v>
       </c>
-      <c r="H39" s="5">
-        <v>3</v>
+      <c r="H39" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I39" s="51" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J39" s="51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3316,7 +3352,7 @@
         <v>24</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D40" s="48">
         <v>3</v>
@@ -3331,14 +3367,14 @@
         <f t="shared" si="4"/>
         <v>16500</v>
       </c>
-      <c r="H40" s="5">
-        <v>3</v>
+      <c r="H40" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I40" s="51" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J40" s="51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3349,7 +3385,7 @@
         <v>24</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D41" s="48">
         <v>2</v>
@@ -3364,14 +3400,14 @@
         <f t="shared" si="4"/>
         <v>11000</v>
       </c>
-      <c r="H41" s="5">
-        <v>2</v>
+      <c r="H41" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I41" s="51" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J41" s="51" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3379,10 +3415,10 @@
         <v>39</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D42" s="48">
         <v>4</v>
@@ -3397,17 +3433,17 @@
         <f>D42*E42</f>
         <v>29200</v>
       </c>
-      <c r="H42" s="5">
-        <v>4</v>
+      <c r="H42" s="5" t="s">
+        <v>254</v>
       </c>
       <c r="I42" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J42" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K42" s="73" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3415,10 +3451,10 @@
         <v>39</v>
       </c>
       <c r="B43" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>116</v>
       </c>
       <c r="D43" s="48">
         <v>3</v>
@@ -3433,17 +3469,17 @@
         <f>D43*E43</f>
         <v>25500</v>
       </c>
-      <c r="H43" s="5">
-        <v>3</v>
+      <c r="H43" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I43" s="51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J43" s="51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K43" s="73" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3451,10 +3487,10 @@
         <v>39</v>
       </c>
       <c r="B44" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="31" t="s">
         <v>94</v>
-      </c>
-      <c r="C44" s="31" t="s">
-        <v>95</v>
       </c>
       <c r="D44" s="48">
         <v>2</v>
@@ -3469,17 +3505,17 @@
         <f>D44*E44</f>
         <v>16000</v>
       </c>
-      <c r="H44" s="5">
-        <v>2</v>
+      <c r="H44" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="I44" s="51" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J44" s="51" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K44" s="73" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3505,17 +3541,17 @@
         <f t="shared" si="4"/>
         <v>21000</v>
       </c>
-      <c r="H45" s="5">
-        <v>3</v>
+      <c r="H45" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I45" s="51" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J45" s="51" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K45" s="73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3541,17 +3577,17 @@
         <f t="shared" si="4"/>
         <v>29500</v>
       </c>
-      <c r="H46" s="5">
-        <v>5</v>
+      <c r="H46" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="I46" s="51" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J46" s="51" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K46" s="73" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3562,7 +3598,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D47" s="48">
         <v>3</v>
@@ -3577,17 +3613,17 @@
         <f t="shared" si="4"/>
         <v>17700</v>
       </c>
-      <c r="H47" s="5">
-        <v>3</v>
+      <c r="H47" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="I47" s="51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J47" s="51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K47" s="73" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3595,10 +3631,10 @@
         <v>39</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D48" s="48">
         <v>2</v>
@@ -3613,14 +3649,14 @@
         <f t="shared" si="4"/>
         <v>11800</v>
       </c>
-      <c r="H48" s="5">
-        <v>2</v>
+      <c r="H48" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="I48" s="51" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J48" s="51" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3628,10 +3664,10 @@
         <v>39</v>
       </c>
       <c r="B49" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="31" t="s">
         <v>61</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>62</v>
       </c>
       <c r="D49" s="48">
         <v>2</v>
@@ -3646,17 +3682,17 @@
         <f t="shared" si="4"/>
         <v>11800</v>
       </c>
-      <c r="H49" s="5">
-        <v>2</v>
+      <c r="H49" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="I49" s="51" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J49" s="51" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K49" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3686,10 +3722,10 @@
         <v>7</v>
       </c>
       <c r="I50" s="51" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J50" s="51" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3715,14 +3751,14 @@
         <f t="shared" si="5"/>
         <v>6000</v>
       </c>
-      <c r="H51" s="5">
-        <v>9</v>
+      <c r="H51" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="I51" s="51" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J51" s="51" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3748,14 +3784,14 @@
         <f t="shared" ref="G52:G55" si="6">D52*E52</f>
         <v>18000</v>
       </c>
-      <c r="H52" s="5">
-        <v>31</v>
+      <c r="H52" s="5" t="s">
+        <v>257</v>
       </c>
       <c r="I52" s="51" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J52" s="51" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3781,14 +3817,14 @@
         <f t="shared" si="6"/>
         <v>66000</v>
       </c>
-      <c r="H53" s="5">
-        <v>31</v>
+      <c r="H53" s="5" t="s">
+        <v>257</v>
       </c>
       <c r="I53" s="51" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J53" s="51" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3799,7 +3835,7 @@
         <v>24</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" s="48">
         <v>1</v>
@@ -3814,14 +3850,14 @@
         <f t="shared" si="6"/>
         <v>14000</v>
       </c>
-      <c r="H54" s="5">
-        <v>23</v>
+      <c r="H54" s="5" t="s">
+        <v>258</v>
       </c>
       <c r="I54" s="51" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J54" s="51" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3851,10 +3887,10 @@
         <v>7</v>
       </c>
       <c r="I55" s="51" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J55" s="51" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3884,10 +3920,10 @@
         <v>7</v>
       </c>
       <c r="I56" s="51" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J56" s="51" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3917,10 +3953,10 @@
         <v>7</v>
       </c>
       <c r="I57" s="51" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J57" s="51" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3931,7 +3967,7 @@
         <v>24</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D58" s="48">
         <v>1</v>
@@ -3950,10 +3986,10 @@
         <v>7</v>
       </c>
       <c r="I58" s="51" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J58" s="51" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3983,10 +4019,10 @@
         <v>7</v>
       </c>
       <c r="I59" s="51" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J59" s="51" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4012,14 +4048,14 @@
         <f t="shared" si="7"/>
         <v>27500</v>
       </c>
-      <c r="H60" s="5">
-        <v>13</v>
+      <c r="H60" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="I60" s="51" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J60" s="51" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4049,21 +4085,21 @@
         <v>7</v>
       </c>
       <c r="I61" s="51" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J61" s="51" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D62" s="48">
         <v>1</v>
@@ -4078,25 +4114,25 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H62" s="5">
-        <v>1</v>
+      <c r="H62" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I62" s="51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J62" s="51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D63" s="48">
         <v>1</v>
@@ -4111,25 +4147,25 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H63" s="5">
-        <v>1</v>
+      <c r="H63" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I63" s="51" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J63" s="51" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D64" s="48">
         <v>1</v>
@@ -4144,25 +4180,25 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H64" s="5">
-        <v>1</v>
+      <c r="H64" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I64" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J64" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D65" s="48">
         <v>1</v>
@@ -4177,25 +4213,25 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H65" s="5">
-        <v>1</v>
+      <c r="H65" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I65" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J65" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D66" s="48">
         <v>1</v>
@@ -4210,25 +4246,25 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H66" s="5">
-        <v>1</v>
+      <c r="H66" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I66" s="51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J66" s="51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D67" s="48">
         <v>1</v>
@@ -4243,25 +4279,25 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H67" s="5">
-        <v>1</v>
+      <c r="H67" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I67" s="51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J67" s="51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D68" s="48">
         <v>1</v>
@@ -4276,25 +4312,25 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H68" s="5">
-        <v>1</v>
+      <c r="H68" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I68" s="51" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J68" s="51" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D69" s="48">
         <v>1</v>
@@ -4309,25 +4345,25 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H69" s="5">
-        <v>1</v>
+      <c r="H69" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I69" s="51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J69" s="51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D70" s="48">
         <v>1</v>
@@ -4342,28 +4378,28 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H70" s="5">
-        <v>1</v>
+      <c r="H70" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I70" s="51" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J70" s="51" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K70" s="73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D71" s="48">
         <v>1</v>
@@ -4378,28 +4414,28 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H71" s="5">
-        <v>1</v>
+      <c r="H71" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I71" s="51" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J71" s="51" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K71" s="73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D72" s="48">
         <v>1</v>
@@ -4414,28 +4450,28 @@
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
-      <c r="H72" s="5">
-        <v>1</v>
+      <c r="H72" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I72" s="51" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J72" s="51" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K72" s="73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B73" s="42" t="s">
         <v>24</v>
       </c>
       <c r="C73" s="43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D73" s="44">
         <v>1</v>
@@ -4450,25 +4486,25 @@
         <f>D73*E73</f>
         <v>5500</v>
       </c>
-      <c r="H73" s="5">
-        <v>1</v>
+      <c r="H73" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I73" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J73" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B74" s="33" t="s">
         <v>24</v>
       </c>
       <c r="C74" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D74" s="35">
         <v>1</v>
@@ -4483,28 +4519,28 @@
         <f>D74*E74</f>
         <v>5500</v>
       </c>
-      <c r="H74" s="5">
-        <v>1</v>
+      <c r="H74" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I74" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J74" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K74" s="73" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D75" s="48">
         <v>1</v>
@@ -4519,28 +4555,28 @@
         <f>D75*E75</f>
         <v>5500</v>
       </c>
-      <c r="H75" s="5">
-        <v>1</v>
+      <c r="H75" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I75" s="51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J75" s="51" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K75" s="73" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D76" s="48">
         <v>1</v>
@@ -4555,28 +4591,28 @@
         <f t="shared" ref="G76" si="8">D76*E76</f>
         <v>5500</v>
       </c>
-      <c r="H76" s="5">
-        <v>1</v>
+      <c r="H76" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I76" s="51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J76" s="51" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K76" s="73" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D77" s="48">
         <v>1</v>
@@ -4585,34 +4621,34 @@
         <v>14000</v>
       </c>
       <c r="F77" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G77" s="49">
         <f t="shared" ref="G77:G78" si="9">D77*E77</f>
         <v>14000</v>
       </c>
-      <c r="H77" s="5">
-        <v>1</v>
+      <c r="H77" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I77" s="51" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J77" s="51" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K77" s="73" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D78" s="48">
         <v>1</v>
@@ -4621,31 +4657,31 @@
         <v>10900</v>
       </c>
       <c r="F78" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G78" s="49">
         <f t="shared" si="9"/>
         <v>10900</v>
       </c>
-      <c r="H78" s="5">
-        <v>1</v>
+      <c r="H78" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I78" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J78" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D79" s="48">
         <v>1</v>
@@ -4660,25 +4696,25 @@
         <f t="shared" ref="G79:G80" si="10">D79*E79</f>
         <v>5500</v>
       </c>
-      <c r="H79" s="5">
-        <v>1</v>
+      <c r="H79" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I79" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J79" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C80" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D80" s="48">
         <v>1</v>
@@ -4693,25 +4729,25 @@
         <f t="shared" si="10"/>
         <v>5500</v>
       </c>
-      <c r="H80" s="5">
-        <v>1</v>
+      <c r="H80" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I80" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J80" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C81" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D81" s="48">
         <v>1</v>
@@ -4726,25 +4762,25 @@
         <f t="shared" ref="G81:G90" si="11">D81*E81</f>
         <v>5500</v>
       </c>
-      <c r="H81" s="5">
-        <v>1</v>
+      <c r="H81" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I81" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J81" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C82" s="38" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D82" s="35">
         <v>1</v>
@@ -4759,25 +4795,25 @@
         <f t="shared" si="11"/>
         <v>5500</v>
       </c>
-      <c r="H82" s="37">
-        <v>1</v>
+      <c r="H82" s="37" t="s">
+        <v>259</v>
       </c>
       <c r="I82" s="75" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J82" s="75" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C83" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D83" s="48">
         <v>1</v>
@@ -4792,25 +4828,25 @@
         <f t="shared" si="11"/>
         <v>7500</v>
       </c>
-      <c r="H83" s="5">
-        <v>1</v>
+      <c r="H83" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I83" s="51" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J83" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C84" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D84" s="48">
         <v>1</v>
@@ -4819,34 +4855,34 @@
         <v>10000</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G84" s="49">
         <f t="shared" si="11"/>
         <v>10000</v>
       </c>
-      <c r="H84" s="5">
-        <v>1</v>
+      <c r="H84" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I84" s="51" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J84" s="51" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K84" s="73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C85" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D85" s="48">
         <v>1</v>
@@ -4855,34 +4891,34 @@
         <v>10000</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G85" s="49">
         <f t="shared" si="11"/>
         <v>10000</v>
       </c>
-      <c r="H85" s="5">
-        <v>1</v>
+      <c r="H85" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I85" s="51" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J85" s="51" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K85" s="73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C86" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D86" s="48">
         <v>1</v>
@@ -4897,25 +4933,25 @@
         <f t="shared" si="11"/>
         <v>10500</v>
       </c>
-      <c r="H86" s="5">
-        <v>1</v>
+      <c r="H86" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I86" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J86" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D87" s="48">
         <v>1</v>
@@ -4930,25 +4966,25 @@
         <f t="shared" si="11"/>
         <v>10500</v>
       </c>
-      <c r="H87" s="5">
-        <v>1</v>
+      <c r="H87" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I87" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J87" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C88" s="31" t="s">
         <v>64</v>
-      </c>
-      <c r="B88" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C88" s="31" t="s">
-        <v>65</v>
       </c>
       <c r="D88" s="48">
         <v>1</v>
@@ -4963,25 +4999,25 @@
         <f t="shared" si="11"/>
         <v>11450</v>
       </c>
-      <c r="H88" s="5">
-        <v>1</v>
+      <c r="H88" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I88" s="51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J88" s="51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B89" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C89" s="32" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D89" s="24">
         <v>1</v>
@@ -4996,28 +5032,28 @@
         <f t="shared" ref="G89" si="12">D89*E89</f>
         <v>5900</v>
       </c>
-      <c r="H89" s="26">
-        <v>1</v>
+      <c r="H89" s="26" t="s">
+        <v>259</v>
       </c>
       <c r="I89" s="51" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J89" s="51" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K89" s="73" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B90" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C90" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D90" s="24">
         <v>1</v>
@@ -5032,28 +5068,28 @@
         <f t="shared" si="11"/>
         <v>9000</v>
       </c>
-      <c r="H90" s="26">
-        <v>1</v>
+      <c r="H90" s="26" t="s">
+        <v>259</v>
       </c>
       <c r="I90" s="51" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J90" s="51" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K90" s="73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B91" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C91" s="32" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D91" s="24">
         <v>1</v>
@@ -5068,28 +5104,28 @@
         <f t="shared" ref="G91" si="13">D91*E91</f>
         <v>9000</v>
       </c>
-      <c r="H91" s="26">
-        <v>1</v>
+      <c r="H91" s="26" t="s">
+        <v>259</v>
       </c>
       <c r="I91" s="51" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J91" s="51" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K91" s="73" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B92" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D92" s="48">
         <v>1</v>
@@ -5104,28 +5140,28 @@
         <f>D92*E92</f>
         <v>5500</v>
       </c>
-      <c r="H92" s="5">
-        <v>1</v>
+      <c r="H92" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I92" s="51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J92" s="51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K92" s="73" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B93" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C93" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D93" s="48">
         <v>1</v>
@@ -5140,25 +5176,25 @@
         <f>D93*E93</f>
         <v>5500</v>
       </c>
-      <c r="H93" s="5">
-        <v>1</v>
+      <c r="H93" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I93" s="51" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J93" s="51" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B94" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C94" s="31" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D94" s="48">
         <v>1</v>
@@ -5167,23 +5203,23 @@
         <v>12000</v>
       </c>
       <c r="F94" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G94" s="49">
         <f t="shared" ref="G94" si="14">D94*E94</f>
         <v>12000</v>
       </c>
-      <c r="H94" s="5">
-        <v>1</v>
+      <c r="H94" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="I94" s="51" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J94" s="51" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K94" s="73" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5200,7 +5236,7 @@
         <v>0</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>2</v>
@@ -5209,13 +5245,13 @@
         <v>3</v>
       </c>
       <c r="H95" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I95" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J95" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -5274,8 +5310,8 @@
         <v>C6 = 23</v>
       </c>
       <c r="H97" s="56" t="str">
-        <f>"En publicación = " &amp; COUNTA(H2:H7,H15:H18,H20:H24,H9:H12,H50,H55:H59,H61,)</f>
-        <v>En publicación = 27</v>
+        <f>"En publicacion = " &amp; COUNTA(H2:H7,H15:H18,H20:H24,H9:H12,H50,H55:H59,H61,)</f>
+        <v>En publicacion = 27</v>
       </c>
       <c r="I97" s="57" t="str">
         <f>"C6 = " &amp; SUM(D15:D21,D30:D32,D49,D53:D59,D79:D83)</f>
@@ -5314,9 +5350,9 @@
         <f>"B6x2 = " &amp; COUNTA(F77:F78,F94)</f>
         <v>B6x2 = 3</v>
       </c>
-      <c r="I99" s="30" t="str">
-        <f>"A5 color = " &amp; SUM(D87,D22)</f>
-        <v>A5 color = 6</v>
+      <c r="I99" s="28" t="str">
+        <f>"B6x2 = " &amp; SUM(D77:D78,D94)</f>
+        <v>B6x2 = 3</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
@@ -5325,12 +5361,12 @@
         <v>Ovni Press = 3</v>
       </c>
       <c r="F100" s="29" t="str">
-        <f>"C6 = " &amp; COUNTA(F84:F85)</f>
-        <v>C6 = 2</v>
-      </c>
-      <c r="I100" s="28" t="str">
-        <f>"B6x2 = " &amp; SUM(D77:D78,D94)</f>
-        <v>B6x2 = 3</v>
+        <f>"C6x2 = " &amp; COUNTA(F84:F85)</f>
+        <v>C6x2 = 2</v>
+      </c>
+      <c r="I100" s="29" t="str">
+        <f>"C6x2 = " &amp; SUM(D84:D85)</f>
+        <v>C6x2 = 2</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
@@ -5342,9 +5378,9 @@
         <f>"A5 color = " &amp; COUNTA(F87,F22)</f>
         <v>A5 color = 2</v>
       </c>
-      <c r="I101" s="29" t="str">
-        <f>"C6x2 = " &amp; SUM(D84:D85)</f>
-        <v>C6x2 = 2</v>
+      <c r="I101" s="30" t="str">
+        <f>"A5 color = " &amp; SUM(D87,D22)</f>
+        <v>A5 color = 6</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
@@ -5403,5 +5439,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="I100" formulaRange="1"/>
+    <ignoredError sqref="F96" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios de vista en el filtro
</commit_message>
<xml_diff>
--- a/assets/Mangas.xlsx
+++ b/assets/Mangas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahue\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62429EE-83EA-4445-9E1F-088DC8C0C980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB05446A-BA1D-4AD8-BAB9-61FDA813AF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6765F00-11DB-40F5-BC3F-F1F6DA2C76AC}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Tomos</t>
   </si>
   <si>
-    <t>Pecio</t>
-  </si>
-  <si>
     <t>Tamaño</t>
   </si>
   <si>
@@ -805,6 +802,9 @@
   </si>
   <si>
     <t>Finalizado</t>
+  </si>
+  <si>
+    <t>Precio</t>
   </si>
 </sst>
 </file>
@@ -1960,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD5DF50-6FBC-4F7F-9AF4-AF00221DFCCC}">
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H96" sqref="H96"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,48 +1982,48 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>3</v>
-      </c>
       <c r="H1" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I1" s="81" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J1" s="81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K1" s="81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="48">
         <v>19</v>
@@ -2032,34 +2032,34 @@
         <v>6000</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" s="49">
         <f t="shared" ref="G2:G13" si="0">D2*E2</f>
         <v>114000</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K2" s="73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="48">
         <v>20</v>
@@ -2068,34 +2068,34 @@
         <v>6000</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" s="49">
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K3" s="74" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="48">
         <v>13</v>
@@ -2104,34 +2104,34 @@
         <v>6000</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" s="49">
         <f t="shared" si="0"/>
         <v>78000</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K4" s="73" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="48">
         <v>13</v>
@@ -2140,34 +2140,34 @@
         <v>6000</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="49">
         <f t="shared" si="0"/>
         <v>78000</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" s="51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J5" s="51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K5" s="73" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="48">
         <v>8</v>
@@ -2176,34 +2176,34 @@
         <v>6000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6" s="49">
         <f t="shared" si="0"/>
         <v>48000</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I6" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J6" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K6" s="73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="48">
         <v>10</v>
@@ -2212,31 +2212,31 @@
         <v>6000</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G7" s="49">
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I7" s="51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="48">
         <v>6</v>
@@ -2245,31 +2245,31 @@
         <v>6000</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G8" s="49">
         <f t="shared" si="0"/>
         <v>36000</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J8" s="51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9" s="48">
         <v>3</v>
@@ -2278,34 +2278,34 @@
         <v>8000</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" s="49">
         <f t="shared" si="0"/>
         <v>24000</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I9" s="51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="73" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" s="48">
         <v>2</v>
@@ -2314,34 +2314,34 @@
         <v>6000</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10" s="49">
         <f t="shared" si="0"/>
         <v>12000</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I10" s="51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J10" s="51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K10" s="73" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="48">
         <v>10</v>
@@ -2350,31 +2350,31 @@
         <v>5500</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G11" s="49">
         <f t="shared" si="0"/>
         <v>55000</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I11" s="51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J11" s="51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="48">
         <v>5</v>
@@ -2383,34 +2383,34 @@
         <v>5500</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G12" s="49">
         <f t="shared" si="0"/>
         <v>27500</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I12" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J12" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K12" s="73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D13" s="48">
         <v>5</v>
@@ -2419,34 +2419,34 @@
         <v>5500</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13" s="49">
         <f t="shared" si="0"/>
         <v>27500</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I13" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J13" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K13" s="73" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D14" s="48">
         <v>2</v>
@@ -2455,34 +2455,34 @@
         <v>6900</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G14" s="49">
         <f t="shared" ref="G14:G28" si="1">D14*E14</f>
         <v>13800</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I14" s="51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J14" s="51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K14" s="73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" s="48">
         <v>12</v>
@@ -2491,34 +2491,34 @@
         <v>5500</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" s="49">
         <f t="shared" si="1"/>
         <v>66000</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I15" s="51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J15" s="51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K15" s="73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="48">
         <v>18</v>
@@ -2527,34 +2527,34 @@
         <v>5500</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" s="49">
         <f t="shared" si="1"/>
         <v>99000</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I16" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J16" s="51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K16" s="73" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="48">
         <v>15</v>
@@ -2563,31 +2563,31 @@
         <v>5500</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" s="49">
         <f t="shared" si="1"/>
         <v>82500</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I17" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J17" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="48">
         <v>9</v>
@@ -2596,34 +2596,34 @@
         <v>5500</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" s="49">
         <f t="shared" si="1"/>
         <v>49500</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I18" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J18" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K18" s="73" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="48">
         <v>8</v>
@@ -2632,34 +2632,34 @@
         <v>5500</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" s="49">
         <f t="shared" si="1"/>
         <v>44000</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I19" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J19" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K19" s="73" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="48">
         <v>8</v>
@@ -2668,34 +2668,34 @@
         <v>5500</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20" s="49">
         <f t="shared" si="1"/>
         <v>44000</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I20" s="51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J20" s="51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K20" s="73" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D21" s="48">
         <v>4</v>
@@ -2704,34 +2704,34 @@
         <v>5500</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21" s="49">
         <f t="shared" si="1"/>
         <v>22000</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I21" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J21" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K21" s="73" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="48">
         <v>5</v>
@@ -2740,34 +2740,34 @@
         <v>20000</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" s="49">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I22" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="J22" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="J22" s="51" t="s">
-        <v>145</v>
-      </c>
       <c r="K22" s="73" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" s="48">
         <v>11</v>
@@ -2776,31 +2776,31 @@
         <v>7500</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="49">
         <f t="shared" si="1"/>
         <v>82500</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I23" s="51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J23" s="51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D24" s="48">
         <v>4</v>
@@ -2809,34 +2809,34 @@
         <v>6900</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G24" s="49">
         <f t="shared" si="1"/>
         <v>27600</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J24" s="51" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K24" s="73" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D25" s="48">
         <v>1</v>
@@ -2845,34 +2845,34 @@
         <v>9800</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G25" s="49">
         <f t="shared" ref="G25" si="2">D25*E25</f>
         <v>9800</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I25" s="51" t="s">
+        <v>240</v>
+      </c>
+      <c r="J25" s="51" t="s">
+        <v>240</v>
+      </c>
+      <c r="K25" s="73" t="s">
         <v>241</v>
-      </c>
-      <c r="J25" s="51" t="s">
-        <v>241</v>
-      </c>
-      <c r="K25" s="73" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D26" s="48">
         <v>1</v>
@@ -2881,34 +2881,34 @@
         <v>12000</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G26" s="49">
         <f t="shared" si="1"/>
         <v>12000</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I26" s="51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J26" s="51" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K26" s="73" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" s="48">
         <v>28</v>
@@ -2917,34 +2917,34 @@
         <v>6000</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G27" s="49">
         <f t="shared" si="1"/>
         <v>168000</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I27" s="51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J27" s="51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K27" s="72" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="77" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D28" s="35">
         <v>2</v>
@@ -2953,31 +2953,31 @@
         <v>6000</v>
       </c>
       <c r="F28" s="39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G28" s="36">
         <f t="shared" si="1"/>
         <v>12000</v>
       </c>
       <c r="H28" s="37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I28" s="75" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J28" s="75" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D29" s="48">
         <v>2</v>
@@ -2986,34 +2986,34 @@
         <v>6000</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G29" s="49">
         <f t="shared" ref="G29" si="3">D29*E29</f>
         <v>12000</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I29" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="J29" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="J29" s="51" t="s">
+      <c r="K29" s="73" t="s">
         <v>208</v>
-      </c>
-      <c r="K29" s="73" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="48">
         <v>23</v>
@@ -3022,31 +3022,31 @@
         <v>5500</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G30" s="49">
         <f t="shared" ref="G30:G49" si="4">D30*E30</f>
         <v>126500</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I30" s="51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J30" s="51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" s="48">
         <v>12</v>
@@ -3055,31 +3055,31 @@
         <v>5500</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G31" s="49">
         <f t="shared" si="4"/>
         <v>66000</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I31" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J31" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="31" t="s">
         <v>24</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>25</v>
       </c>
       <c r="D32" s="48">
         <v>8</v>
@@ -3088,34 +3088,34 @@
         <v>5500</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G32" s="49">
         <f>D32*E32</f>
         <v>44000</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I32" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J32" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K32" s="73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D33" s="48">
         <v>2</v>
@@ -3124,34 +3124,34 @@
         <v>5500</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G33" s="49">
         <f t="shared" si="4"/>
         <v>11000</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I33" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J33" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K33" s="73" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D34" s="48">
         <v>3</v>
@@ -3160,34 +3160,34 @@
         <v>5500</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G34" s="49">
         <f t="shared" si="4"/>
         <v>16500</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I34" s="51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J34" s="51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K34" s="73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D35" s="48">
         <v>13</v>
@@ -3196,31 +3196,31 @@
         <v>5500</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G35" s="49">
         <f t="shared" si="4"/>
         <v>71500</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I35" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J35" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" s="48">
         <v>8</v>
@@ -3229,31 +3229,31 @@
         <v>5500</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G36" s="49">
         <f t="shared" si="4"/>
         <v>44000</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I36" s="51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J36" s="51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D37" s="48">
         <v>4</v>
@@ -3262,31 +3262,31 @@
         <v>5500</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G37" s="49">
         <f t="shared" si="4"/>
         <v>22000</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I37" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="J37" s="51" t="s">
         <v>155</v>
-      </c>
-      <c r="J37" s="51" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="48">
         <v>3</v>
@@ -3295,31 +3295,31 @@
         <v>5500</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G38" s="49">
         <f t="shared" si="4"/>
         <v>16500</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I38" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J38" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D39" s="48">
         <v>3</v>
@@ -3328,31 +3328,31 @@
         <v>5500</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G39" s="49">
         <f t="shared" si="4"/>
         <v>16500</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I39" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J39" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D40" s="48">
         <v>3</v>
@@ -3361,31 +3361,31 @@
         <v>5500</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G40" s="49">
         <f t="shared" si="4"/>
         <v>16500</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I40" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J40" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D41" s="48">
         <v>2</v>
@@ -3394,31 +3394,31 @@
         <v>5500</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G41" s="49">
         <f t="shared" si="4"/>
         <v>11000</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I41" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="J41" s="51" t="s">
         <v>158</v>
-      </c>
-      <c r="J41" s="51" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D42" s="48">
         <v>4</v>
@@ -3427,34 +3427,34 @@
         <v>7300</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G42" s="49">
         <f>D42*E42</f>
         <v>29200</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I42" s="51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J42" s="51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K42" s="73" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D43" s="48">
         <v>3</v>
@@ -3463,34 +3463,34 @@
         <v>8500</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G43" s="49">
         <f>D43*E43</f>
         <v>25500</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I43" s="51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J43" s="51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K43" s="73" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="31" t="s">
         <v>93</v>
-      </c>
-      <c r="C44" s="31" t="s">
-        <v>94</v>
       </c>
       <c r="D44" s="48">
         <v>2</v>
@@ -3499,34 +3499,34 @@
         <v>8000</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G44" s="49">
         <f>D44*E44</f>
         <v>16000</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I44" s="51" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J44" s="51" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K44" s="73" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="31" t="s">
         <v>34</v>
-      </c>
-      <c r="C45" s="31" t="s">
-        <v>35</v>
       </c>
       <c r="D45" s="48">
         <v>3</v>
@@ -3535,34 +3535,34 @@
         <v>7000</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G45" s="49">
         <f t="shared" si="4"/>
         <v>21000</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I45" s="51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J45" s="51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K45" s="73" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="31" t="s">
         <v>28</v>
-      </c>
-      <c r="C46" s="31" t="s">
-        <v>29</v>
       </c>
       <c r="D46" s="48">
         <v>5</v>
@@ -3571,34 +3571,34 @@
         <v>5900</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G46" s="49">
         <f t="shared" si="4"/>
         <v>29500</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I46" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="J46" s="51" t="s">
         <v>161</v>
       </c>
-      <c r="J46" s="51" t="s">
-        <v>162</v>
-      </c>
       <c r="K46" s="73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D47" s="48">
         <v>3</v>
@@ -3607,34 +3607,34 @@
         <v>5900</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G47" s="49">
         <f t="shared" si="4"/>
         <v>17700</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I47" s="51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J47" s="51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K47" s="73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D48" s="48">
         <v>2</v>
@@ -3643,31 +3643,31 @@
         <v>5900</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G48" s="49">
         <f t="shared" si="4"/>
         <v>11800</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I48" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J48" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B49" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="31" t="s">
         <v>60</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>61</v>
       </c>
       <c r="D49" s="48">
         <v>2</v>
@@ -3676,34 +3676,34 @@
         <v>5900</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G49" s="49">
         <f t="shared" si="4"/>
         <v>11800</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I49" s="51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J49" s="51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K49" s="73" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="31" t="s">
         <v>40</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="31" t="s">
-        <v>41</v>
       </c>
       <c r="D50" s="48">
         <v>2</v>
@@ -3712,31 +3712,31 @@
         <v>6000</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G50" s="49">
         <f t="shared" ref="G50:G72" si="5">D50*E50</f>
         <v>12000</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I50" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J50" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D51" s="48">
         <v>1</v>
@@ -3745,31 +3745,31 @@
         <v>6000</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G51" s="49">
         <f t="shared" si="5"/>
         <v>6000</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I51" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J51" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D52" s="48">
         <v>3</v>
@@ -3778,31 +3778,31 @@
         <v>6000</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G52" s="49">
         <f t="shared" ref="G52:G55" si="6">D52*E52</f>
         <v>18000</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I52" s="51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J52" s="51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D53" s="48">
         <v>12</v>
@@ -3811,31 +3811,31 @@
         <v>5500</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G53" s="49">
         <f t="shared" si="6"/>
         <v>66000</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I53" s="51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J53" s="51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D54" s="48">
         <v>1</v>
@@ -3844,31 +3844,31 @@
         <v>14000</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G54" s="49">
         <f t="shared" si="6"/>
         <v>14000</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I54" s="51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J54" s="51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D55" s="48">
         <v>6</v>
@@ -3877,31 +3877,31 @@
         <v>5500</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G55" s="49">
         <f t="shared" si="6"/>
         <v>33000</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I55" s="51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J55" s="51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D56" s="48">
         <v>4</v>
@@ -3910,31 +3910,31 @@
         <v>5500</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G56" s="49">
         <f t="shared" ref="G56:G61" si="7">D56*E56</f>
         <v>22000</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I56" s="51" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J56" s="51" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D57" s="48">
         <v>5</v>
@@ -3943,31 +3943,31 @@
         <v>5500</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G57" s="49">
         <f t="shared" si="7"/>
         <v>27500</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I57" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J57" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D58" s="48">
         <v>1</v>
@@ -3976,31 +3976,31 @@
         <v>5500</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G58" s="49">
         <f t="shared" si="7"/>
         <v>5500</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I58" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J58" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D59" s="48">
         <v>1</v>
@@ -4009,31 +4009,31 @@
         <v>5500</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G59" s="49">
         <f t="shared" si="7"/>
         <v>5500</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I59" s="51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J59" s="51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D60" s="48">
         <v>5</v>
@@ -4042,31 +4042,31 @@
         <v>5500</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G60" s="49">
         <f t="shared" si="7"/>
         <v>27500</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I60" s="51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J60" s="51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D61" s="48">
         <v>1</v>
@@ -4075,31 +4075,31 @@
         <v>5500</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G61" s="49">
         <f t="shared" si="7"/>
         <v>5500</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I61" s="51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J61" s="51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D62" s="48">
         <v>1</v>
@@ -4108,31 +4108,31 @@
         <v>5500</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G62" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I62" s="51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J62" s="51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D63" s="48">
         <v>1</v>
@@ -4141,31 +4141,31 @@
         <v>5500</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G63" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I63" s="51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J63" s="51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D64" s="48">
         <v>1</v>
@@ -4174,31 +4174,31 @@
         <v>5500</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G64" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I64" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J64" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D65" s="48">
         <v>1</v>
@@ -4207,31 +4207,31 @@
         <v>5500</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G65" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I65" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J65" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D66" s="48">
         <v>1</v>
@@ -4240,31 +4240,31 @@
         <v>5500</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G66" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I66" s="51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J66" s="51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D67" s="48">
         <v>1</v>
@@ -4273,31 +4273,31 @@
         <v>5500</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G67" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I67" s="51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J67" s="51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D68" s="48">
         <v>1</v>
@@ -4306,31 +4306,31 @@
         <v>5500</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G68" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I68" s="51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J68" s="51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D69" s="48">
         <v>1</v>
@@ -4339,31 +4339,31 @@
         <v>5500</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G69" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I69" s="51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J69" s="51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D70" s="48">
         <v>1</v>
@@ -4372,34 +4372,34 @@
         <v>5500</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G70" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I70" s="51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J70" s="51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K70" s="73" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D71" s="48">
         <v>1</v>
@@ -4408,34 +4408,34 @@
         <v>5500</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G71" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I71" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J71" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K71" s="73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D72" s="48">
         <v>1</v>
@@ -4444,34 +4444,34 @@
         <v>5500</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G72" s="49">
         <f t="shared" si="5"/>
         <v>5500</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I72" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J72" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K72" s="73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B73" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C73" s="43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D73" s="44">
         <v>1</v>
@@ -4480,31 +4480,31 @@
         <v>5500</v>
       </c>
       <c r="F73" s="46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G73" s="47">
         <f>D73*E73</f>
         <v>5500</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I73" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J73" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B74" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C74" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D74" s="35">
         <v>1</v>
@@ -4513,34 +4513,34 @@
         <v>5500</v>
       </c>
       <c r="F74" s="39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G74" s="36">
         <f>D74*E74</f>
         <v>5500</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I74" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J74" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K74" s="73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D75" s="48">
         <v>1</v>
@@ -4549,34 +4549,34 @@
         <v>5500</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G75" s="49">
         <f>D75*E75</f>
         <v>5500</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I75" s="51" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J75" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K75" s="73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D76" s="48">
         <v>1</v>
@@ -4585,34 +4585,34 @@
         <v>5500</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G76" s="49">
         <f t="shared" ref="G76" si="8">D76*E76</f>
         <v>5500</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I76" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="J76" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J76" s="51" t="s">
-        <v>200</v>
-      </c>
       <c r="K76" s="73" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D77" s="48">
         <v>1</v>
@@ -4621,34 +4621,34 @@
         <v>14000</v>
       </c>
       <c r="F77" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G77" s="49">
         <f t="shared" ref="G77:G78" si="9">D77*E77</f>
         <v>14000</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I77" s="51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J77" s="51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K77" s="73" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D78" s="48">
         <v>1</v>
@@ -4657,31 +4657,31 @@
         <v>10900</v>
       </c>
       <c r="F78" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G78" s="49">
         <f t="shared" si="9"/>
         <v>10900</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I78" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J78" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D79" s="48">
         <v>1</v>
@@ -4690,31 +4690,31 @@
         <v>5500</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G79" s="49">
         <f t="shared" ref="G79:G80" si="10">D79*E79</f>
         <v>5500</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I79" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J79" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C80" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D80" s="48">
         <v>1</v>
@@ -4723,31 +4723,31 @@
         <v>5500</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G80" s="49">
         <f t="shared" si="10"/>
         <v>5500</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I80" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J80" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C81" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D81" s="48">
         <v>1</v>
@@ -4756,31 +4756,31 @@
         <v>5500</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G81" s="49">
         <f t="shared" ref="G81:G90" si="11">D81*E81</f>
         <v>5500</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I81" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J81" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C82" s="38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D82" s="35">
         <v>1</v>
@@ -4789,31 +4789,31 @@
         <v>5500</v>
       </c>
       <c r="F82" s="39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G82" s="36">
         <f t="shared" si="11"/>
         <v>5500</v>
       </c>
       <c r="H82" s="37" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I82" s="75" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J82" s="75" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C83" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D83" s="48">
         <v>1</v>
@@ -4822,31 +4822,31 @@
         <v>7500</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G83" s="49">
         <f t="shared" si="11"/>
         <v>7500</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I83" s="51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J83" s="51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C84" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D84" s="48">
         <v>1</v>
@@ -4855,34 +4855,34 @@
         <v>10000</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G84" s="49">
         <f t="shared" si="11"/>
         <v>10000</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I84" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J84" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K84" s="73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C85" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D85" s="48">
         <v>1</v>
@@ -4891,34 +4891,34 @@
         <v>10000</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G85" s="49">
         <f t="shared" si="11"/>
         <v>10000</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I85" s="51" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J85" s="51" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K85" s="73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C86" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D86" s="48">
         <v>1</v>
@@ -4927,31 +4927,31 @@
         <v>10500</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G86" s="49">
         <f t="shared" si="11"/>
         <v>10500</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I86" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J86" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D87" s="48">
         <v>1</v>
@@ -4960,31 +4960,31 @@
         <v>10500</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G87" s="49">
         <f t="shared" si="11"/>
         <v>10500</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I87" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J87" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C88" s="31" t="s">
         <v>63</v>
-      </c>
-      <c r="B88" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C88" s="31" t="s">
-        <v>64</v>
       </c>
       <c r="D88" s="48">
         <v>1</v>
@@ -4993,31 +4993,31 @@
         <v>11450</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G88" s="49">
         <f t="shared" si="11"/>
         <v>11450</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I88" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J88" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C89" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D89" s="24">
         <v>1</v>
@@ -5026,34 +5026,34 @@
         <v>5900</v>
       </c>
       <c r="F89" s="78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G89" s="25">
         <f t="shared" ref="G89" si="12">D89*E89</f>
         <v>5900</v>
       </c>
       <c r="H89" s="26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I89" s="51" t="s">
+        <v>202</v>
+      </c>
+      <c r="J89" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="J89" s="51" t="s">
-        <v>204</v>
-      </c>
       <c r="K89" s="73" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C90" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D90" s="24">
         <v>1</v>
@@ -5062,34 +5062,34 @@
         <v>9000</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G90" s="25">
         <f t="shared" si="11"/>
         <v>9000</v>
       </c>
       <c r="H90" s="26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I90" s="51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J90" s="51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K90" s="73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C91" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D91" s="24">
         <v>1</v>
@@ -5098,34 +5098,34 @@
         <v>9000</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G91" s="25">
         <f t="shared" ref="G91" si="13">D91*E91</f>
         <v>9000</v>
       </c>
       <c r="H91" s="26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I91" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J91" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K91" s="73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D92" s="48">
         <v>1</v>
@@ -5134,34 +5134,34 @@
         <v>5500</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G92" s="49">
         <f>D92*E92</f>
         <v>5500</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I92" s="51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J92" s="51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K92" s="73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C93" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D93" s="48">
         <v>1</v>
@@ -5170,31 +5170,31 @@
         <v>5500</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G93" s="49">
         <f>D93*E93</f>
         <v>5500</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I93" s="51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J93" s="51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B94" s="79" t="s">
+        <v>218</v>
+      </c>
+      <c r="C94" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="C94" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="D94" s="48">
         <v>1</v>
@@ -5203,55 +5203,55 @@
         <v>12000</v>
       </c>
       <c r="F94" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G94" s="49">
         <f t="shared" ref="G94" si="14">D94*E94</f>
         <v>12000</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I94" s="51" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J94" s="51" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K94" s="73" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D95" s="12" t="s">
         <v>0</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F95" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G95" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G95" s="12" t="s">
-        <v>3</v>
-      </c>
       <c r="H95" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I95" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J95" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cambios en el filtro
</commit_message>
<xml_diff>
--- a/assets/Mangas.xlsx
+++ b/assets/Mangas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahue\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB05446A-BA1D-4AD8-BAB9-61FDA813AF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A2304E-2498-472A-8F7D-592CE0C538F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6765F00-11DB-40F5-BC3F-F1F6DA2C76AC}"/>
   </bookViews>
@@ -1328,7 +1328,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1575,9 +1575,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1960,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD5DF50-6FBC-4F7F-9AF4-AF00221DFCCC}">
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5284,8 +5281,8 @@
         <v>2627950</v>
       </c>
       <c r="H96" s="55" t="str">
-        <f>"Finalizados = " &amp; COUNTA(H8,H13:H14,H19,H25:H49,,H51:H54,H60,H62:H94)</f>
-        <v>Finalizados = 68</v>
+        <f>"Finalizados = " &amp; COUNTA(H8,H13:H14,H19,H25:H49,H51:H54,H60,H62:H94)</f>
+        <v>Finalizados = 67</v>
       </c>
       <c r="I96" s="54" t="str">
         <f>"B6 = " &amp; SUM(D2:D14,D24,D27:D29,D33:D42,D46:D48,D50:D52,D60:D76,D88,D90:D93)</f>
@@ -5296,7 +5293,7 @@
         <v>Series = 46</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="60" t="str">
         <f>"Completado = " &amp; COUNTA(A27:A49)</f>
         <v>Completado = 23</v>
@@ -5310,16 +5307,15 @@
         <v>C6 = 23</v>
       </c>
       <c r="H97" s="56" t="str">
-        <f>"En publicacion = " &amp; COUNTA(H2:H7,H15:H18,H20:H24,H9:H12,H50,H55:H59,H61,)</f>
-        <v>En publicacion = 27</v>
+        <f>"En publicacion = " &amp; COUNTA(H2:H7,H9:H12,H15:H18,H20:H24,H50,H55:H59,H61)</f>
+        <v>En publicacion = 26</v>
       </c>
       <c r="I97" s="57" t="str">
         <f>"C6 = " &amp; SUM(D15:D21,D30:D32,D49,D53:D59,D79:D83)</f>
         <v>C6 = 154</v>
       </c>
-      <c r="J97" s="83"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="61" t="str">
         <f>"Droppeado = " &amp; COUNTA(A50:A61)</f>
         <v>Droppeado = 12</v>
@@ -5337,7 +5333,7 @@
         <v>A5 = 23</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="62" t="str">
         <f>"Tomo único = " &amp; COUNTA(A62:A94)</f>
         <v>Tomo único = 33</v>
@@ -5355,7 +5351,7 @@
         <v>B6x2 = 3</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B100" s="67" t="str">
         <f>"Ovni Press = " &amp; COUNTA(B24,B90:B91)</f>
         <v>Ovni Press = 3</v>
@@ -5369,7 +5365,7 @@
         <v>C6x2 = 2</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B101" s="69" t="str">
         <f>"Planeta Cómic = " &amp; COUNTA(B25:B26,B42:B43)</f>
         <v>Planeta Cómic = 4</v>
@@ -5383,25 +5379,25 @@
         <v>A5 color = 6</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B102" s="68" t="str">
         <f>"Utopia = " &amp; COUNTA(B48:B49)</f>
         <v>Utopia = 2</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B103" s="70" t="str">
         <f>"Merci = " &amp; COUNTA(B44)</f>
         <v>Merci = 1</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B104" s="71" t="str">
         <f>"Milky Way = " &amp; COUNTA(B88)</f>
         <v>Milky Way = 1</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B105" s="80" t="str">
         <f>"Moztros = " &amp; COUNTA(B94)</f>
         <v>Moztros = 1</v>

</xml_diff>

<commit_message>
actualizado excel de mangas
</commit_message>
<xml_diff>
--- a/assets/Mangas.xlsx
+++ b/assets/Mangas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahue\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahue\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A2304E-2498-472A-8F7D-592CE0C538F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E0CD24-2D97-4B8F-85DC-2194271CC660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6765F00-11DB-40F5-BC3F-F1F6DA2C76AC}"/>
   </bookViews>
@@ -1957,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD5DF50-6FBC-4F7F-9AF4-AF00221DFCCC}">
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,7 +2023,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="48">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="49">
         <v>6000</v>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="G2" s="49">
         <f t="shared" ref="G2:G13" si="0">D2*E2</f>
-        <v>114000</v>
+        <v>120000</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>6</v>
@@ -2203,7 +2203,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="48">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="49">
         <v>6000</v>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="G7" s="49">
         <f t="shared" si="0"/>
-        <v>60000</v>
+        <v>66000</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>6</v>
@@ -2341,7 +2341,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="48">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="49">
         <v>5500</v>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="G11" s="49">
         <f t="shared" si="0"/>
-        <v>55000</v>
+        <v>60500</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>6</v>
@@ -2410,7 +2410,7 @@
         <v>100</v>
       </c>
       <c r="D13" s="48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" s="49">
         <v>5500</v>
@@ -2420,7 +2420,7 @@
       </c>
       <c r="G13" s="49">
         <f t="shared" si="0"/>
-        <v>27500</v>
+        <v>33000</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>246</v>
@@ -2836,7 +2836,7 @@
         <v>239</v>
       </c>
       <c r="D25" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="49">
         <v>9800</v>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="G25" s="49">
         <f t="shared" ref="G25" si="2">D25*E25</f>
-        <v>9800</v>
+        <v>19600</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>247</v>
@@ -5266,7 +5266,7 @@
       </c>
       <c r="D96" s="52">
         <f>SUM(D2:D94)</f>
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="E96" s="53">
         <f>SUM(E2:E94)</f>
@@ -5278,7 +5278,7 @@
       </c>
       <c r="G96" s="53">
         <f>SUM(G2:G94)</f>
-        <v>2627950</v>
+        <v>2660750</v>
       </c>
       <c r="H96" s="55" t="str">
         <f>"Finalizados = " &amp; COUNTA(H8,H13:H14,H19,H25:H49,H51:H54,H60,H62:H94)</f>
@@ -5286,7 +5286,7 @@
       </c>
       <c r="I96" s="54" t="str">
         <f>"B6 = " &amp; SUM(D2:D14,D24,D27:D29,D33:D42,D46:D48,D50:D52,D60:D76,D88,D90:D93)</f>
-        <v>B6 = 239</v>
+        <v>B6 = 243</v>
       </c>
       <c r="J96" s="82" t="str">
         <f>"Series = " &amp; COUNTA(K2:K6,K9:K10,K12:K16,K18:K22,K24:K27,K29,K32:K34,K42:K47,K49,K70:K72,K74:K77,K84:K85,K89:K92,K94)</f>
@@ -5330,7 +5330,7 @@
       </c>
       <c r="I98" s="27" t="str">
         <f>"A5 = " &amp; SUM(D23,D25:D26,D43:D45,D86,D89)</f>
-        <v>A5 = 23</v>
+        <v>A5 = 24</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Subido excel automatico utilizando Google Sheet y mejorados tanto los filtros como el codigo en general
</commit_message>
<xml_diff>
--- a/assets/Mangas.xlsx
+++ b/assets/Mangas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahue\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D97200-012C-4276-A837-06582063D62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCE02A3-EA32-4AE5-8CC7-5CDE28390024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6765F00-11DB-40F5-BC3F-F1F6DA2C76AC}"/>
   </bookViews>
@@ -1627,10 +1627,10 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD5DF50-6FBC-4F7F-9AF4-AF00221DFCCC}">
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H103" sqref="H103"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I103" sqref="I103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2026,7 +2026,7 @@
     <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
@@ -5692,17 +5692,17 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30 F32:F100 F25:F28 F9:F23">
+  <conditionalFormatting sqref="F9:F23 F25:F28 F30 F32:F100">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"C6"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30 F32:F100 F9:F28">
+  <conditionalFormatting sqref="F9:F28 F30 F32:F100">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"A5"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H30 H32:H100 H3:H28">
+  <conditionalFormatting sqref="H3:H28 H30 H32:H100">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En publicacion">
       <formula>NOT(ISERROR(SEARCH("En publicacion",H3)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mejorado el README, arreglados los filtros y actualizada la coleccion
</commit_message>
<xml_diff>
--- a/assets/Mangas.xlsx
+++ b/assets/Mangas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/44df28c8ac89212a/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="6_{EDABB7A8-8D17-44E7-9064-82807FFB5D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64264E85-5ED2-4F59-8B81-47EA1EE3F704}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="6_{EDABB7A8-8D17-44E7-9064-82807FFB5D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{997AB341-FE1B-4DF8-9F22-2B2CADD088A2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1728,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H120" sqref="H120"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H121" sqref="H121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5911,8 +5911,8 @@
         <v>C6 = 28</v>
       </c>
       <c r="H120" s="9" t="str">
-        <f>"Finalizados+H120 = " &amp; COUNTA(H6,H12,H19,H26:H27,H29:H54,H56:H59,H65,H67:H117)</f>
-        <v>Finalizados+H120 = 87</v>
+        <f>"En publicación = " &amp; COUNTA(H2:H5,H7:H11,H13:H18,H20:H25,H28,H55,H60:H64,H66)</f>
+        <v>En publicación = 29</v>
       </c>
       <c r="I120" s="43" t="str">
         <f>"C6 = " &amp; SUM(D14:D22,D34:D36,D54,D58:D64,D89:D96)</f>

</xml_diff>

<commit_message>
Actualizados precios y nuevos mangas
</commit_message>
<xml_diff>
--- a/assets/Mangas.xlsx
+++ b/assets/Mangas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\proyectos\Mangas\mangas\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4F7207-7112-46D0-8551-8C5379E6C3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08E7404-B93C-4EEF-A3F5-A8567004071E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="324">
   <si>
     <t>Estado</t>
   </si>
@@ -906,9 +906,6 @@
     <t>Spy x Family - 11 al 14</t>
   </si>
   <si>
-    <t>Gachiakuta - 2 al 8</t>
-  </si>
-  <si>
     <t>Kibook Ediciones</t>
   </si>
   <si>
@@ -921,9 +918,6 @@
     <t>Obaru</t>
   </si>
   <si>
-    <t>Blue Lock - 13 al 29</t>
-  </si>
-  <si>
     <t>Hikaru Ga Shinda Natsu - 2 al 5</t>
   </si>
   <si>
@@ -939,9 +933,6 @@
     <t>The Blue Summer and You #2</t>
   </si>
   <si>
-    <t>Blue Lock : Episode Nagi - 1 al 5</t>
-  </si>
-  <si>
     <t>Historias de Sexo de Chicas JK</t>
   </si>
   <si>
@@ -954,9 +945,6 @@
     <t>Sakamoto Days - 3 al 15</t>
   </si>
   <si>
-    <t>Dandadan - 8 al 15</t>
-  </si>
-  <si>
     <t>Houseki no Kuni - 3 al 8</t>
   </si>
   <si>
@@ -991,6 +979,30 @@
   </si>
   <si>
     <t>Moyori Mori</t>
+  </si>
+  <si>
+    <t>Dandadan - 8 al 16</t>
+  </si>
+  <si>
+    <t>Blue Lock - 13 al 30</t>
+  </si>
+  <si>
+    <t>Blue Lock : Episode Nagi - 1 al 6</t>
+  </si>
+  <si>
+    <t>Gachiakuta - 2 al 9</t>
+  </si>
+  <si>
+    <t>Adaban</t>
+  </si>
+  <si>
+    <t>Dai Tezuka</t>
+  </si>
+  <si>
+    <t>NON</t>
+  </si>
+  <si>
+    <t>Adaban - 1</t>
   </si>
 </sst>
 </file>
@@ -1486,7 +1498,71 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0066"/>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF3333CC"/>
+          <bgColor rgb="FF3333CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0EAE02"/>
+          <bgColor rgb="FF0EAE02"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0066"/>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF3333CC"/>
+          <bgColor rgb="FF3333CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0EAE02"/>
+          <bgColor rgb="FF0EAE02"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1855,7 +1931,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C129"/>
+      <selection activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1928,7 +2004,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="7">
-        <f t="shared" ref="G2:G128" si="0">D2*E2</f>
+        <f t="shared" ref="G2:G129" si="0">D2*E2</f>
         <v>253000</v>
       </c>
       <c r="H2" s="44" t="s">
@@ -1941,7 +2017,7 @@
         <v>14</v>
       </c>
       <c r="K2" s="41" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2030,14 +2106,14 @@
         <v>18</v>
       </c>
       <c r="E5" s="7">
-        <v>9000</v>
+        <v>11000</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" si="0"/>
-        <v>162000</v>
+        <v>198000</v>
       </c>
       <c r="H5" s="44" t="s">
         <v>274</v>
@@ -2096,29 +2172,32 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E7" s="7">
-        <v>11000</v>
+        <v>10500</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>110000</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>183</v>
+        <v>31500</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>274</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="K7" s="41" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2129,32 +2208,32 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D8" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" s="7">
-        <v>10500</v>
+        <v>12500</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="0"/>
-        <v>31500</v>
+        <v>62500</v>
       </c>
       <c r="H8" s="44" t="s">
         <v>274</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K8" s="41" t="s">
-        <v>29</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2165,32 +2244,32 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="6">
+        <v>91</v>
+      </c>
+      <c r="D9" s="11">
         <v>5</v>
       </c>
       <c r="E9" s="7">
-        <v>12500</v>
+        <v>11000</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="7">
-        <f t="shared" si="0"/>
-        <v>62500</v>
+        <f>D9*E9</f>
+        <v>55000</v>
       </c>
       <c r="H9" s="44" t="s">
         <v>274</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="K9" s="41" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2201,32 +2280,32 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>312</v>
       </c>
       <c r="D10" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E10" s="7">
-        <v>11000</v>
+        <v>12000</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="7">
         <f>D10*E10</f>
-        <v>55000</v>
+        <v>24000</v>
       </c>
       <c r="H10" s="44" t="s">
         <v>274</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>92</v>
+        <v>311</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>93</v>
+        <v>311</v>
       </c>
       <c r="K10" s="41" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2237,104 +2316,104 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D11" s="11">
+        <v>32</v>
+      </c>
+      <c r="D11" s="6">
         <v>1</v>
       </c>
       <c r="E11" s="7">
-        <v>11000</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>13</v>
+        <v>13000</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="G11" s="7">
-        <f>D11*E11</f>
-        <v>11000</v>
+        <f t="shared" si="0"/>
+        <v>13000</v>
       </c>
       <c r="H11" s="44" t="s">
         <v>274</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>315</v>
+        <v>34</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>315</v>
+        <v>34</v>
       </c>
       <c r="K11" s="41" t="s">
-        <v>317</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>11</v>
+      <c r="B12" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="D12" s="11">
+        <v>7</v>
       </c>
       <c r="E12" s="7">
-        <v>13000</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>33</v>
+        <v>8900</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="G12" s="7">
         <f t="shared" si="0"/>
-        <v>13000</v>
+        <v>62300</v>
       </c>
       <c r="H12" s="44" t="s">
         <v>274</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="K12" s="41" t="s">
-        <v>35</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D13" s="11">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E13" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="7">
-        <f t="shared" si="0"/>
-        <v>59500</v>
+        <f t="shared" ref="G13" si="1">D13*E13</f>
+        <v>44500</v>
       </c>
       <c r="H13" s="44" t="s">
         <v>274</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>41</v>
+      <c r="I13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="K13" s="41" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2345,32 +2424,32 @@
         <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>320</v>
       </c>
       <c r="D14" s="11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E14" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="7">
         <f t="shared" si="0"/>
-        <v>42500</v>
+        <v>8900</v>
       </c>
       <c r="H14" s="44" t="s">
         <v>274</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>45</v>
+        <v>321</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>45</v>
+        <v>322</v>
       </c>
       <c r="K14" s="41" t="s">
-        <v>283</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2387,14 +2466,14 @@
         <v>14</v>
       </c>
       <c r="E15" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="0"/>
-        <v>105000</v>
+        <v>119000</v>
       </c>
       <c r="H15" s="44" t="s">
         <v>274</v>
@@ -2420,17 +2499,17 @@
         <v>49</v>
       </c>
       <c r="D16" s="11">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E16" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G16" s="7">
-        <f t="shared" ref="G16" si="1">D16*E16</f>
-        <v>217500</v>
+        <f t="shared" ref="G16" si="2">D16*E16</f>
+        <v>255000</v>
       </c>
       <c r="H16" s="44" t="s">
         <v>274</v>
@@ -2442,7 +2521,7 @@
         <v>51</v>
       </c>
       <c r="K16" s="41" t="s">
-        <v>296</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2456,17 +2535,17 @@
         <v>265</v>
       </c>
       <c r="D17" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E17" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" si="0"/>
-        <v>37500</v>
+        <v>51000</v>
       </c>
       <c r="H17" s="44" t="s">
         <v>274</v>
@@ -2478,7 +2557,7 @@
         <v>51</v>
       </c>
       <c r="K17" s="41" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2528,14 +2607,14 @@
         <v>15</v>
       </c>
       <c r="E19" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="0"/>
-        <v>112500</v>
+        <v>127500</v>
       </c>
       <c r="H19" s="44" t="s">
         <v>274</v>
@@ -2547,7 +2626,7 @@
         <v>55</v>
       </c>
       <c r="K19" s="41" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2561,17 +2640,17 @@
         <v>58</v>
       </c>
       <c r="D20" s="11">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E20" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G20" s="7">
         <f t="shared" si="0"/>
-        <v>112500</v>
+        <v>136000</v>
       </c>
       <c r="H20" s="44" t="s">
         <v>274</v>
@@ -2583,7 +2662,7 @@
         <v>59</v>
       </c>
       <c r="K20" s="41" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2597,17 +2676,17 @@
         <v>60</v>
       </c>
       <c r="D21" s="11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G21" s="7">
         <f t="shared" si="0"/>
-        <v>60000</v>
+        <v>76500</v>
       </c>
       <c r="H21" s="44" t="s">
         <v>274</v>
@@ -2619,7 +2698,7 @@
         <v>61</v>
       </c>
       <c r="K21" s="41" t="s">
-        <v>291</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2636,14 +2715,14 @@
         <v>3</v>
       </c>
       <c r="E22" s="7">
-        <v>7500</v>
+        <v>8900</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G22" s="7">
-        <f t="shared" ref="G22" si="2">D22*E22</f>
-        <v>22500</v>
+        <f t="shared" ref="G22" si="3">D22*E22</f>
+        <v>26700</v>
       </c>
       <c r="H22" s="44" t="s">
         <v>274</v>
@@ -2655,7 +2734,7 @@
         <v>64</v>
       </c>
       <c r="K22" s="41" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2666,20 +2745,20 @@
         <v>36</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D23" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" si="0"/>
-        <v>22500</v>
+        <v>17000</v>
       </c>
       <c r="H23" s="44" t="s">
         <v>274</v>
@@ -2691,7 +2770,7 @@
         <v>106</v>
       </c>
       <c r="K23" s="41" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2705,17 +2784,17 @@
         <v>65</v>
       </c>
       <c r="D24" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E24" s="7">
-        <v>22500</v>
+        <v>23900</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>66</v>
       </c>
       <c r="G24" s="7">
         <f t="shared" si="0"/>
-        <v>202500</v>
+        <v>239000</v>
       </c>
       <c r="H24" s="44" t="s">
         <v>274</v>
@@ -2727,7 +2806,7 @@
         <v>68</v>
       </c>
       <c r="K24" s="41" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2744,14 +2823,14 @@
         <v>13</v>
       </c>
       <c r="E25" s="7">
-        <v>9000</v>
+        <v>10900</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G25" s="7">
         <f t="shared" si="0"/>
-        <v>117000</v>
+        <v>141700</v>
       </c>
       <c r="H25" s="44" t="s">
         <v>274</v>
@@ -2777,14 +2856,14 @@
         <v>8</v>
       </c>
       <c r="E26" s="7">
-        <v>11000</v>
+        <v>12000</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="7">
         <f t="shared" si="0"/>
-        <v>88000</v>
+        <v>96000</v>
       </c>
       <c r="H26" s="44" t="s">
         <v>274</v>
@@ -2796,7 +2875,7 @@
         <v>73</v>
       </c>
       <c r="K26" s="41" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2813,14 +2892,14 @@
         <v>2</v>
       </c>
       <c r="E27" s="7">
-        <v>15400</v>
+        <v>16600</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G27" s="7">
         <f t="shared" si="0"/>
-        <v>30800</v>
+        <v>33200</v>
       </c>
       <c r="H27" s="13" t="s">
         <v>183</v>
@@ -2832,7 +2911,7 @@
         <v>76</v>
       </c>
       <c r="K27" s="41" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2875,72 +2954,72 @@
       <c r="A29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="34" t="s">
-        <v>258</v>
+      <c r="B29" s="19" t="s">
+        <v>80</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>309</v>
+        <v>81</v>
       </c>
       <c r="D29" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="7">
-        <v>18900</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>33</v>
+        <v>32000</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="G29" s="7">
-        <f>D29*E29</f>
-        <v>56700</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>183</v>
+        <f t="shared" si="0"/>
+        <v>64000</v>
+      </c>
+      <c r="H29" s="44" t="s">
+        <v>274</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>260</v>
+        <v>82</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>260</v>
+        <v>82</v>
       </c>
       <c r="K29" s="41" t="s">
-        <v>310</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>80</v>
+      <c r="A30" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D30" s="6">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E30" s="7">
-        <v>32000</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>66</v>
+        <v>12500</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="G30" s="7">
         <f t="shared" si="0"/>
-        <v>64000</v>
-      </c>
-      <c r="H30" s="44" t="s">
-        <v>274</v>
+        <v>350000</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="K30" s="41" t="s">
-        <v>280</v>
+        <v>38</v>
+      </c>
+      <c r="K30" s="42" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2951,32 +3030,29 @@
         <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="D31" s="6">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E31" s="7">
-        <v>12500</v>
+        <v>11000</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="7">
-        <f t="shared" si="0"/>
-        <v>350000</v>
+        <f>D31*E31</f>
+        <v>143000</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="K31" s="42" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3098,14 +3174,14 @@
         <v>23</v>
       </c>
       <c r="E35" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G35" s="7">
         <f t="shared" si="0"/>
-        <v>172500</v>
+        <v>195500</v>
       </c>
       <c r="H35" s="13" t="s">
         <v>183</v>
@@ -3131,14 +3207,14 @@
         <v>12</v>
       </c>
       <c r="E36" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G36" s="7">
         <f t="shared" si="0"/>
-        <v>90000</v>
+        <v>102000</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>183</v>
@@ -3164,14 +3240,14 @@
         <v>8</v>
       </c>
       <c r="E37" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G37" s="7">
         <f t="shared" si="0"/>
-        <v>60000</v>
+        <v>68000</v>
       </c>
       <c r="H37" s="13" t="s">
         <v>183</v>
@@ -3200,14 +3276,14 @@
         <v>11</v>
       </c>
       <c r="E38" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G38" s="7">
         <f>D38*E38</f>
-        <v>82500</v>
+        <v>93500</v>
       </c>
       <c r="H38" s="13" t="s">
         <v>183</v>
@@ -3236,14 +3312,14 @@
         <v>12</v>
       </c>
       <c r="E39" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G39" s="7">
         <f>D39*E39</f>
-        <v>102000</v>
+        <v>106800</v>
       </c>
       <c r="H39" s="13" t="s">
         <v>183</v>
@@ -3255,7 +3331,7 @@
         <v>43</v>
       </c>
       <c r="K39" s="41" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3272,14 +3348,14 @@
         <v>16</v>
       </c>
       <c r="E40" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G40" s="7">
         <f>D40*E40</f>
-        <v>136000</v>
+        <v>142400</v>
       </c>
       <c r="H40" s="13" t="s">
         <v>183</v>
@@ -3291,7 +3367,7 @@
         <v>39</v>
       </c>
       <c r="K40" s="41" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3308,14 +3384,14 @@
         <v>2</v>
       </c>
       <c r="E41" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="7">
         <f t="shared" si="0"/>
-        <v>17000</v>
+        <v>17800</v>
       </c>
       <c r="H41" s="13" t="s">
         <v>183</v>
@@ -3344,14 +3420,14 @@
         <v>3</v>
       </c>
       <c r="E42" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G42" s="7">
         <f t="shared" si="0"/>
-        <v>25500</v>
+        <v>26700</v>
       </c>
       <c r="H42" s="13" t="s">
         <v>183</v>
@@ -3380,14 +3456,14 @@
         <v>3</v>
       </c>
       <c r="E43" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="7">
         <f t="shared" si="0"/>
-        <v>25500</v>
+        <v>26700</v>
       </c>
       <c r="H43" s="13" t="s">
         <v>183</v>
@@ -3416,14 +3492,14 @@
         <v>13</v>
       </c>
       <c r="E44" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G44" s="7">
         <f t="shared" si="0"/>
-        <v>110500</v>
+        <v>115700</v>
       </c>
       <c r="H44" s="13" t="s">
         <v>183</v>
@@ -3449,14 +3525,14 @@
         <v>8</v>
       </c>
       <c r="E45" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G45" s="7">
         <f t="shared" si="0"/>
-        <v>68000</v>
+        <v>71200</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>183</v>
@@ -3482,14 +3558,14 @@
         <v>4</v>
       </c>
       <c r="E46" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G46" s="7">
         <f t="shared" si="0"/>
-        <v>34000</v>
+        <v>35600</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>183</v>
@@ -3515,14 +3591,14 @@
         <v>3</v>
       </c>
       <c r="E47" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G47" s="7">
         <f t="shared" si="0"/>
-        <v>25500</v>
+        <v>26700</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>183</v>
@@ -3548,14 +3624,14 @@
         <v>3</v>
       </c>
       <c r="E48" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G48" s="7">
         <f t="shared" si="0"/>
-        <v>25500</v>
+        <v>26700</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>183</v>
@@ -3581,14 +3657,14 @@
         <v>3</v>
       </c>
       <c r="E49" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="7">
         <f t="shared" si="0"/>
-        <v>25500</v>
+        <v>26700</v>
       </c>
       <c r="H49" s="13" t="s">
         <v>183</v>
@@ -3614,14 +3690,14 @@
         <v>2</v>
       </c>
       <c r="E50" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="7">
-        <f t="shared" ref="G50" si="3">D50*E50</f>
-        <v>17000</v>
+        <f t="shared" ref="G50" si="4">D50*E50</f>
+        <v>17800</v>
       </c>
       <c r="H50" s="13" t="s">
         <v>183</v>
@@ -3647,14 +3723,14 @@
         <v>3</v>
       </c>
       <c r="E51" s="7">
-        <v>7166</v>
+        <v>7500</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="7">
         <f>D51*E51</f>
-        <v>21498</v>
+        <v>22500</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>183</v>
@@ -3680,14 +3756,14 @@
         <v>4</v>
       </c>
       <c r="E52" s="7">
-        <v>12300</v>
+        <v>14900</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="7">
         <f t="shared" si="0"/>
-        <v>49200</v>
+        <v>59600</v>
       </c>
       <c r="H52" s="13" t="s">
         <v>183</v>
@@ -3716,14 +3792,14 @@
         <v>5</v>
       </c>
       <c r="E53" s="7">
-        <v>13300</v>
+        <v>14100</v>
       </c>
       <c r="F53" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G53" s="7">
         <f t="shared" si="0"/>
-        <v>66500</v>
+        <v>70500</v>
       </c>
       <c r="H53" s="13" t="s">
         <v>183</v>
@@ -3778,72 +3854,72 @@
       <c r="A55" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B55" s="22" t="s">
-        <v>137</v>
+      <c r="B55" s="34" t="s">
+        <v>258</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>138</v>
+        <v>305</v>
       </c>
       <c r="D55" s="6">
         <v>3</v>
       </c>
       <c r="E55" s="7">
-        <v>12500</v>
+        <v>18900</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G55" s="7">
-        <f t="shared" si="0"/>
-        <v>37500</v>
+        <f>D55*E55</f>
+        <v>56700</v>
       </c>
       <c r="H55" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>139</v>
+        <v>260</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>139</v>
+        <v>260</v>
       </c>
       <c r="K55" s="41" t="s">
-        <v>140</v>
+        <v>306</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B56" s="23" t="s">
-        <v>141</v>
+      <c r="B56" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D56" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E56" s="7">
-        <v>8900</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>13</v>
+        <v>13500</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="G56" s="7">
         <f t="shared" si="0"/>
-        <v>44500</v>
+        <v>40500</v>
       </c>
       <c r="H56" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="K56" s="41" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3854,65 +3930,68 @@
         <v>141</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D57" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E57" s="7">
-        <v>8900</v>
+        <v>11900</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G57" s="7">
         <f t="shared" si="0"/>
-        <v>26700</v>
+        <v>59500</v>
       </c>
       <c r="H57" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K57" s="41" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B58" s="24" t="s">
-        <v>149</v>
+      <c r="B58" s="23" t="s">
+        <v>141</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D58" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E58" s="7">
-        <v>9000</v>
+        <v>11900</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G58" s="7">
         <f t="shared" si="0"/>
-        <v>18000</v>
+        <v>35700</v>
       </c>
       <c r="H58" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>151</v>
+        <v>147</v>
+      </c>
+      <c r="K58" s="41" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3923,7 +4002,7 @@
         <v>149</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D59" s="6">
         <v>2</v>
@@ -3932,7 +4011,7 @@
         <v>9000</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="G59" s="7">
         <f t="shared" si="0"/>
@@ -3942,46 +4021,46 @@
         <v>183</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="K59" s="41" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>11</v>
+      <c r="A60" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>149</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D60" s="6">
         <v>2</v>
       </c>
       <c r="E60" s="7">
-        <v>12000</v>
+        <v>9000</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="G60" s="7">
         <f t="shared" si="0"/>
-        <v>24000</v>
-      </c>
-      <c r="H60" s="44" t="s">
-        <v>274</v>
+        <v>18000</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>157</v>
+        <v>153</v>
+      </c>
+      <c r="K60" s="41" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3992,29 +4071,29 @@
         <v>11</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D61" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" s="7">
-        <v>11000</v>
+        <v>12000</v>
       </c>
       <c r="F61" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G61" s="7">
         <f t="shared" si="0"/>
-        <v>11000</v>
-      </c>
-      <c r="H61" s="13" t="s">
-        <v>183</v>
+        <v>24000</v>
+      </c>
+      <c r="H61" s="44" t="s">
+        <v>274</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4025,62 +4104,62 @@
         <v>11</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D62" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E62" s="7">
-        <v>12500</v>
+        <v>11000</v>
       </c>
       <c r="F62" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G62" s="7">
         <f t="shared" si="0"/>
-        <v>37500</v>
+        <v>11000</v>
       </c>
       <c r="H62" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="B63" s="14" t="s">
-        <v>36</v>
+      <c r="B63" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D63" s="6">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E63" s="7">
-        <v>7500</v>
+        <v>12500</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="G63" s="7">
         <f t="shared" si="0"/>
-        <v>90000</v>
+        <v>37500</v>
       </c>
       <c r="H63" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4091,29 +4170,29 @@
         <v>36</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D64" s="6">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E64" s="7">
-        <v>17700</v>
+        <v>7500</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G64" s="7">
         <f t="shared" si="0"/>
-        <v>17700</v>
+        <v>90000</v>
       </c>
       <c r="H64" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4124,29 +4203,29 @@
         <v>36</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D65" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E65" s="7">
-        <v>7500</v>
+        <v>17700</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G65" s="7">
         <f t="shared" si="0"/>
-        <v>45000</v>
-      </c>
-      <c r="H65" s="44" t="s">
-        <v>274</v>
+        <v>17700</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4157,29 +4236,29 @@
         <v>36</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D66" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E66" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G66" s="7">
         <f t="shared" si="0"/>
-        <v>30000</v>
+        <v>51000</v>
       </c>
       <c r="H66" s="44" t="s">
         <v>274</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4190,29 +4269,29 @@
         <v>36</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D67" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E67" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G67" s="7">
         <f t="shared" si="0"/>
-        <v>37500</v>
+        <v>34000</v>
       </c>
       <c r="H67" s="44" t="s">
         <v>274</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4223,29 +4302,29 @@
         <v>36</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D68" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E68" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F68" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G68" s="7">
         <f t="shared" si="0"/>
-        <v>7500</v>
+        <v>42500</v>
       </c>
       <c r="H68" s="44" t="s">
         <v>274</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4256,29 +4335,29 @@
         <v>36</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D69" s="6">
         <v>1</v>
       </c>
       <c r="E69" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G69" s="7">
         <f t="shared" si="0"/>
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="H69" s="44" t="s">
         <v>274</v>
       </c>
       <c r="I69" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4289,29 +4368,29 @@
         <v>36</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D70" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E70" s="7">
         <v>8500</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="G70" s="7">
         <f t="shared" si="0"/>
-        <v>42500</v>
-      </c>
-      <c r="H70" s="13" t="s">
-        <v>183</v>
+        <v>8500</v>
+      </c>
+      <c r="H70" s="44" t="s">
+        <v>274</v>
       </c>
       <c r="I70" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4322,98 +4401,98 @@
         <v>36</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D71" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E71" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F71" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G71" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
-      </c>
-      <c r="H71" s="44" t="s">
+        <v>44500</v>
+      </c>
+      <c r="H71" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J71" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D72" s="6">
+        <v>1</v>
+      </c>
+      <c r="E72" s="7">
+        <v>8900</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G72" s="7">
+        <f t="shared" si="0"/>
+        <v>8900</v>
+      </c>
+      <c r="H72" s="44" t="s">
         <v>274</v>
       </c>
-      <c r="I71" s="10" t="s">
+      <c r="I72" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="J71" s="10" t="s">
+      <c r="J72" s="10" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="B72" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D72" s="11">
-        <v>1</v>
-      </c>
-      <c r="E72" s="7">
-        <v>18000</v>
-      </c>
-      <c r="F72" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G72" s="7">
-        <f t="shared" si="0"/>
-        <v>18000</v>
-      </c>
-      <c r="H72" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="I72" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J72" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K72" s="41" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B73" s="14" t="s">
-        <v>36</v>
+      <c r="B73" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D73" s="6">
+        <v>182</v>
+      </c>
+      <c r="D73" s="11">
         <v>1</v>
       </c>
       <c r="E73" s="7">
-        <v>8500</v>
-      </c>
-      <c r="F73" s="8" t="s">
+        <v>18000</v>
+      </c>
+      <c r="F73" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G73" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>18000</v>
       </c>
       <c r="H73" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I73" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J73" s="10" t="s">
-        <v>39</v>
+      <c r="I73" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J73" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K73" s="41" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4424,29 +4503,29 @@
         <v>36</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D74" s="6">
         <v>1</v>
       </c>
       <c r="E74" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F74" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G74" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H74" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I74" s="10" t="s">
-        <v>186</v>
+        <v>39</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>186</v>
+        <v>39</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4457,29 +4536,29 @@
         <v>36</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D75" s="6">
         <v>1</v>
       </c>
       <c r="E75" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F75" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G75" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H75" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I75" s="10" t="s">
-        <v>43</v>
+        <v>186</v>
       </c>
       <c r="J75" s="10" t="s">
-        <v>43</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4490,29 +4569,29 @@
         <v>36</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D76" s="6">
         <v>1</v>
       </c>
       <c r="E76" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F76" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G76" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H76" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I76" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4523,29 +4602,29 @@
         <v>36</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D77" s="6">
         <v>1</v>
       </c>
       <c r="E77" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G77" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H77" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I77" s="10" t="s">
-        <v>190</v>
+        <v>45</v>
       </c>
       <c r="J77" s="10" t="s">
-        <v>190</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4556,20 +4635,20 @@
         <v>36</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D78" s="6">
         <v>1</v>
       </c>
       <c r="E78" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G78" s="7">
-        <f t="shared" ref="G78" si="4">D78*E78</f>
-        <v>8500</v>
+        <f t="shared" si="0"/>
+        <v>8900</v>
       </c>
       <c r="H78" s="13" t="s">
         <v>183</v>
@@ -4589,20 +4668,20 @@
         <v>36</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>301</v>
+        <v>191</v>
       </c>
       <c r="D79" s="6">
         <v>1</v>
       </c>
       <c r="E79" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F79" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G79" s="7">
-        <f t="shared" si="0"/>
-        <v>8500</v>
+        <f t="shared" ref="G79" si="5">D79*E79</f>
+        <v>8900</v>
       </c>
       <c r="H79" s="13" t="s">
         <v>183</v>
@@ -4622,29 +4701,29 @@
         <v>36</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>192</v>
+        <v>299</v>
       </c>
       <c r="D80" s="6">
         <v>1</v>
       </c>
       <c r="E80" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F80" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G80" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H80" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I80" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4655,29 +4734,29 @@
         <v>36</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D81" s="6">
         <v>1</v>
       </c>
       <c r="E81" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F81" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G81" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H81" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I81" s="10" t="s">
-        <v>109</v>
+        <v>193</v>
       </c>
       <c r="J81" s="10" t="s">
-        <v>109</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4688,32 +4767,29 @@
         <v>36</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D82" s="6">
         <v>1</v>
       </c>
       <c r="E82" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F82" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G82" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H82" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I82" s="10" t="s">
-        <v>196</v>
+        <v>109</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="K82" s="41" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4724,32 +4800,32 @@
         <v>36</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D83" s="6">
         <v>1</v>
       </c>
       <c r="E83" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F83" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G83" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H83" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I83" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K83" s="41" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4760,20 +4836,20 @@
         <v>36</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D84" s="6">
         <v>1</v>
       </c>
       <c r="E84" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G84" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H84" s="13" t="s">
         <v>183</v>
@@ -4785,7 +4861,7 @@
         <v>198</v>
       </c>
       <c r="K84" s="41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4796,32 +4872,32 @@
         <v>36</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D85" s="6">
         <v>1</v>
       </c>
       <c r="E85" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F85" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G85" s="7">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H85" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I85" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="K85" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4832,32 +4908,32 @@
         <v>36</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D86" s="6">
         <v>1</v>
       </c>
       <c r="E86" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G86" s="7">
-        <f>D86*E86</f>
-        <v>8500</v>
+        <f t="shared" si="0"/>
+        <v>8900</v>
       </c>
       <c r="H86" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I86" s="10" t="s">
-        <v>43</v>
+        <v>201</v>
       </c>
       <c r="J86" s="10" t="s">
-        <v>43</v>
+        <v>202</v>
       </c>
       <c r="K86" s="41" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4868,32 +4944,32 @@
         <v>36</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D87" s="6">
         <v>1</v>
       </c>
       <c r="E87" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G87" s="7">
         <f>D87*E87</f>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H87" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I87" s="10" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="J87" s="10" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="K87" s="41" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4904,32 +4980,32 @@
         <v>36</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D88" s="6">
         <v>1</v>
       </c>
       <c r="E88" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F88" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G88" s="7">
         <f>D88*E88</f>
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="H88" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I88" s="10" t="s">
-        <v>206</v>
+        <v>63</v>
       </c>
       <c r="J88" s="10" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="K88" s="41" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4940,20 +5016,20 @@
         <v>36</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D89" s="6">
         <v>1</v>
       </c>
       <c r="E89" s="7">
-        <v>8500</v>
+        <v>8900</v>
       </c>
       <c r="F89" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G89" s="7">
-        <f t="shared" ref="G89" si="5">D89*E89</f>
-        <v>8500</v>
+        <f>D89*E89</f>
+        <v>8900</v>
       </c>
       <c r="H89" s="13" t="s">
         <v>183</v>
@@ -4962,10 +5038,10 @@
         <v>206</v>
       </c>
       <c r="J89" s="10" t="s">
-        <v>208</v>
+        <v>16</v>
       </c>
       <c r="K89" s="41" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4976,20 +5052,20 @@
         <v>36</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>267</v>
+        <v>207</v>
       </c>
       <c r="D90" s="6">
         <v>1</v>
       </c>
       <c r="E90" s="7">
-        <v>14900</v>
-      </c>
-      <c r="F90" s="28" t="s">
-        <v>211</v>
+        <v>8900</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="G90" s="7">
-        <f>D90*E90</f>
-        <v>14900</v>
+        <f t="shared" ref="G90" si="6">D90*E90</f>
+        <v>8900</v>
       </c>
       <c r="H90" s="13" t="s">
         <v>183</v>
@@ -4998,10 +5074,10 @@
         <v>206</v>
       </c>
       <c r="J90" s="10" t="s">
-        <v>268</v>
+        <v>208</v>
       </c>
       <c r="K90" s="41" t="s">
-        <v>267</v>
+        <v>207</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5012,32 +5088,32 @@
         <v>36</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>210</v>
+        <v>267</v>
       </c>
       <c r="D91" s="6">
         <v>1</v>
       </c>
       <c r="E91" s="7">
-        <v>18500</v>
+        <v>16900</v>
       </c>
       <c r="F91" s="28" t="s">
         <v>211</v>
       </c>
       <c r="G91" s="7">
         <f>D91*E91</f>
-        <v>18500</v>
+        <v>16900</v>
       </c>
       <c r="H91" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I91" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="J91" s="10" t="s">
-        <v>212</v>
+        <v>268</v>
       </c>
       <c r="K91" s="41" t="s">
-        <v>210</v>
+        <v>267</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5048,32 +5124,32 @@
         <v>36</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D92" s="6">
         <v>1</v>
       </c>
       <c r="E92" s="7">
-        <v>13900</v>
+        <v>19900</v>
       </c>
       <c r="F92" s="28" t="s">
         <v>211</v>
       </c>
       <c r="G92" s="7">
         <f>D92*E92</f>
-        <v>13900</v>
+        <v>19900</v>
       </c>
       <c r="H92" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I92" s="10" t="s">
-        <v>43</v>
+        <v>212</v>
       </c>
       <c r="J92" s="10" t="s">
-        <v>43</v>
+        <v>212</v>
       </c>
       <c r="K92" s="41" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5084,7 +5160,7 @@
         <v>36</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D93" s="6">
         <v>1</v>
@@ -5096,7 +5172,7 @@
         <v>211</v>
       </c>
       <c r="G93" s="7">
-        <f t="shared" ref="G93" si="6">D93*E93</f>
+        <f>D93*E93</f>
         <v>14900</v>
       </c>
       <c r="H93" s="13" t="s">
@@ -5107,6 +5183,9 @@
       </c>
       <c r="J93" s="10" t="s">
         <v>43</v>
+      </c>
+      <c r="K93" s="41" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5117,32 +5196,29 @@
         <v>36</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>278</v>
+        <v>214</v>
       </c>
       <c r="D94" s="6">
         <v>1</v>
       </c>
       <c r="E94" s="7">
-        <v>13900</v>
+        <v>15900</v>
       </c>
       <c r="F94" s="28" t="s">
         <v>211</v>
       </c>
       <c r="G94" s="7">
-        <f>D94*E94</f>
-        <v>13900</v>
+        <f t="shared" ref="G94" si="7">D94*E94</f>
+        <v>15900</v>
       </c>
       <c r="H94" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I94" s="10" t="s">
-        <v>279</v>
+        <v>43</v>
       </c>
       <c r="J94" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="K94" s="41" t="s">
-        <v>278</v>
+        <v>43</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5153,29 +5229,32 @@
         <v>36</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>203</v>
+        <v>278</v>
       </c>
       <c r="D95" s="6">
         <v>1</v>
       </c>
       <c r="E95" s="7">
-        <v>7500</v>
-      </c>
-      <c r="F95" s="8" t="s">
-        <v>47</v>
+        <v>14900</v>
+      </c>
+      <c r="F95" s="28" t="s">
+        <v>211</v>
       </c>
       <c r="G95" s="7">
         <f>D95*E95</f>
-        <v>7500</v>
+        <v>14900</v>
       </c>
       <c r="H95" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I95" s="10" t="s">
-        <v>53</v>
+        <v>279</v>
       </c>
       <c r="J95" s="10" t="s">
-        <v>53</v>
+        <v>279</v>
+      </c>
+      <c r="K95" s="41" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5186,20 +5265,20 @@
         <v>36</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="D96" s="6">
         <v>1</v>
       </c>
       <c r="E96" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F96" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G96" s="7">
-        <f t="shared" si="0"/>
-        <v>7500</v>
+        <f>D96*E96</f>
+        <v>8500</v>
       </c>
       <c r="H96" s="13" t="s">
         <v>183</v>
@@ -5219,20 +5298,20 @@
         <v>36</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D97" s="6">
         <v>1</v>
       </c>
       <c r="E97" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F97" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G97" s="7">
         <f t="shared" si="0"/>
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="H97" s="13" t="s">
         <v>183</v>
@@ -5248,32 +5327,32 @@
       <c r="A98" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B98" s="15" t="s">
+      <c r="B98" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D98" s="11">
+        <v>216</v>
+      </c>
+      <c r="D98" s="6">
         <v>1</v>
       </c>
       <c r="E98" s="7">
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="F98" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G98" s="7">
         <f t="shared" si="0"/>
-        <v>7500</v>
+        <v>8500</v>
       </c>
       <c r="H98" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I98" s="16" t="s">
+      <c r="I98" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J98" s="16" t="s">
+      <c r="J98" s="10" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5281,36 +5360,33 @@
       <c r="A99" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B99" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D99" s="6">
+        <v>217</v>
+      </c>
+      <c r="D99" s="11">
         <v>1</v>
       </c>
       <c r="E99" s="7">
-        <v>9900</v>
+        <v>8500</v>
       </c>
       <c r="F99" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G99" s="7">
-        <f>D99*E99</f>
-        <v>9900</v>
+        <f t="shared" si="0"/>
+        <v>8500</v>
       </c>
       <c r="H99" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I99" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J99" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="K99" s="41" t="s">
-        <v>266</v>
+      <c r="I99" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J99" s="16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5321,20 +5397,20 @@
         <v>36</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="D100" s="6">
         <v>1</v>
       </c>
       <c r="E100" s="7">
-        <v>9900</v>
+        <v>10900</v>
       </c>
       <c r="F100" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G100" s="7">
         <f>D100*E100</f>
-        <v>9900</v>
+        <v>10900</v>
       </c>
       <c r="H100" s="13" t="s">
         <v>183</v>
@@ -5346,7 +5422,7 @@
         <v>48</v>
       </c>
       <c r="K100" s="41" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
     </row>
     <row r="101" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5357,32 +5433,32 @@
         <v>36</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>218</v>
+        <v>285</v>
       </c>
       <c r="D101" s="6">
         <v>1</v>
       </c>
       <c r="E101" s="7">
-        <v>9900</v>
+        <v>11900</v>
       </c>
       <c r="F101" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G101" s="7">
-        <f t="shared" si="0"/>
-        <v>9900</v>
+        <f>D101*E101</f>
+        <v>11900</v>
       </c>
       <c r="H101" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I101" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J101" s="10" t="s">
-        <v>219</v>
+        <v>48</v>
       </c>
       <c r="K101" s="41" t="s">
-        <v>218</v>
+        <v>285</v>
       </c>
     </row>
     <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5393,29 +5469,32 @@
         <v>36</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D102" s="6">
         <v>1</v>
       </c>
       <c r="E102" s="7">
-        <v>7500</v>
+        <v>10900</v>
       </c>
       <c r="F102" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G102" s="7">
         <f t="shared" si="0"/>
-        <v>7500</v>
+        <v>10900</v>
       </c>
       <c r="H102" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I102" s="10" t="s">
-        <v>221</v>
+        <v>53</v>
       </c>
       <c r="J102" s="10" t="s">
-        <v>222</v>
+        <v>219</v>
+      </c>
+      <c r="K102" s="41" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5426,32 +5505,29 @@
         <v>36</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D103" s="6">
         <v>1</v>
       </c>
       <c r="E103" s="7">
-        <v>8900</v>
+        <v>8500</v>
       </c>
       <c r="F103" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G103" s="7">
         <f t="shared" si="0"/>
-        <v>8900</v>
+        <v>8500</v>
       </c>
       <c r="H103" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I103" s="10" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J103" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="K103" s="41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5462,29 +5538,32 @@
         <v>36</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D104" s="6">
         <v>1</v>
       </c>
       <c r="E104" s="7">
-        <v>9900</v>
-      </c>
-      <c r="F104" s="29" t="s">
+        <v>9500</v>
+      </c>
+      <c r="F104" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G104" s="7">
         <f t="shared" si="0"/>
-        <v>9900</v>
+        <v>9500</v>
       </c>
       <c r="H104" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I104" s="10" t="s">
-        <v>99</v>
+        <v>224</v>
       </c>
       <c r="J104" s="10" t="s">
-        <v>100</v>
+        <v>224</v>
+      </c>
+      <c r="K104" s="41" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5495,32 +5574,29 @@
         <v>36</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D105" s="6">
         <v>1</v>
       </c>
       <c r="E105" s="7">
-        <v>13900</v>
-      </c>
-      <c r="F105" s="30" t="s">
-        <v>227</v>
+        <v>10900</v>
+      </c>
+      <c r="F105" s="29" t="s">
+        <v>47</v>
       </c>
       <c r="G105" s="7">
         <f t="shared" si="0"/>
-        <v>13900</v>
+        <v>10900</v>
       </c>
       <c r="H105" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I105" s="10" t="s">
-        <v>171</v>
+        <v>99</v>
       </c>
       <c r="J105" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="K105" s="41" t="s">
-        <v>226</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5531,68 +5607,68 @@
         <v>36</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D106" s="6">
         <v>1</v>
       </c>
       <c r="E106" s="7">
-        <v>13900</v>
+        <v>13500</v>
       </c>
       <c r="F106" s="30" t="s">
         <v>227</v>
       </c>
       <c r="G106" s="7">
         <f t="shared" si="0"/>
-        <v>13900</v>
+        <v>13500</v>
       </c>
       <c r="H106" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I106" s="10" t="s">
-        <v>229</v>
+        <v>171</v>
       </c>
       <c r="J106" s="10" t="s">
-        <v>229</v>
+        <v>171</v>
       </c>
       <c r="K106" s="41" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D107" s="11">
+        <v>228</v>
+      </c>
+      <c r="D107" s="6">
         <v>1</v>
       </c>
       <c r="E107" s="7">
-        <v>19900</v>
-      </c>
-      <c r="F107" s="31" t="s">
-        <v>33</v>
+        <v>13500</v>
+      </c>
+      <c r="F107" s="30" t="s">
+        <v>227</v>
       </c>
       <c r="G107" s="7">
-        <f>D107*E107</f>
-        <v>19900</v>
+        <f t="shared" si="0"/>
+        <v>13500</v>
       </c>
       <c r="H107" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I107" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="J107" s="16" t="s">
-        <v>43</v>
+      <c r="I107" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="J107" s="10" t="s">
+        <v>229</v>
       </c>
       <c r="K107" s="41" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5603,20 +5679,20 @@
         <v>36</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D108" s="11">
         <v>1</v>
       </c>
       <c r="E108" s="7">
-        <v>19900</v>
+        <v>21500</v>
       </c>
       <c r="F108" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G108" s="7">
-        <f t="shared" si="0"/>
-        <v>19900</v>
+        <f>D108*E108</f>
+        <v>21500</v>
       </c>
       <c r="H108" s="13" t="s">
         <v>183</v>
@@ -5628,7 +5704,7 @@
         <v>43</v>
       </c>
       <c r="K108" s="41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5639,20 +5715,20 @@
         <v>36</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D109" s="11">
         <v>1</v>
       </c>
       <c r="E109" s="7">
-        <v>15500</v>
+        <v>21500</v>
       </c>
       <c r="F109" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G109" s="7">
-        <f>D109*E109</f>
-        <v>15500</v>
+        <f t="shared" si="0"/>
+        <v>21500</v>
       </c>
       <c r="H109" s="13" t="s">
         <v>183</v>
@@ -5664,40 +5740,43 @@
         <v>43</v>
       </c>
       <c r="K109" s="41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B110" s="14" t="s">
+      <c r="B110" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D110" s="6">
+        <v>232</v>
+      </c>
+      <c r="D110" s="11">
         <v>1</v>
       </c>
       <c r="E110" s="7">
-        <v>15500</v>
-      </c>
-      <c r="F110" s="12" t="s">
+        <v>16900</v>
+      </c>
+      <c r="F110" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G110" s="7">
-        <f t="shared" si="0"/>
-        <v>15500</v>
+        <f>D110*E110</f>
+        <v>16900</v>
       </c>
       <c r="H110" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I110" s="10" t="s">
+      <c r="I110" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J110" s="10" t="s">
+      <c r="J110" s="16" t="s">
         <v>43</v>
+      </c>
+      <c r="K110" s="41" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5708,20 +5787,20 @@
         <v>36</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D111" s="6">
         <v>1</v>
       </c>
       <c r="E111" s="7">
-        <v>15500</v>
-      </c>
-      <c r="F111" s="17" t="s">
-        <v>66</v>
+        <v>16900</v>
+      </c>
+      <c r="F111" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="G111" s="7">
         <f t="shared" si="0"/>
-        <v>15500</v>
+        <v>16900</v>
       </c>
       <c r="H111" s="13" t="s">
         <v>183</v>
@@ -5737,196 +5816,193 @@
       <c r="A112" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B112" s="32" t="s">
-        <v>235</v>
+      <c r="B112" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D112" s="6">
         <v>1</v>
       </c>
       <c r="E112" s="7">
-        <v>27000</v>
-      </c>
-      <c r="F112" s="8" t="s">
-        <v>13</v>
+        <v>16900</v>
+      </c>
+      <c r="F112" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="G112" s="7">
         <f t="shared" si="0"/>
-        <v>27000</v>
+        <v>16900</v>
       </c>
       <c r="H112" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I112" s="10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="J112" s="10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="113" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B113" s="23" t="s">
-        <v>141</v>
+      <c r="B113" s="32" t="s">
+        <v>235</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D113" s="6">
         <v>1</v>
       </c>
       <c r="E113" s="7">
-        <v>14900</v>
-      </c>
-      <c r="F113" s="12" t="s">
-        <v>33</v>
+        <v>27000</v>
+      </c>
+      <c r="F113" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="G113" s="7">
-        <f t="shared" ref="G113" si="7">D113*E113</f>
-        <v>14900</v>
+        <f t="shared" si="0"/>
+        <v>27000</v>
       </c>
       <c r="H113" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I113" s="10" t="s">
-        <v>238</v>
+        <v>57</v>
       </c>
       <c r="J113" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="K113" s="41" t="s">
-        <v>237</v>
+        <v>57</v>
       </c>
     </row>
     <row r="114" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B114" s="18" t="s">
-        <v>74</v>
+      <c r="B114" s="23" t="s">
+        <v>141</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>304</v>
+        <v>237</v>
       </c>
       <c r="D114" s="6">
         <v>1</v>
       </c>
       <c r="E114" s="7">
-        <v>17900</v>
+        <v>11900</v>
       </c>
       <c r="F114" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G114" s="7">
-        <f t="shared" si="0"/>
-        <v>17900</v>
+        <f t="shared" ref="G114" si="8">D114*E114</f>
+        <v>11900</v>
       </c>
       <c r="H114" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I114" s="10" t="s">
-        <v>76</v>
+        <v>238</v>
       </c>
       <c r="J114" s="10" t="s">
-        <v>76</v>
+        <v>239</v>
       </c>
       <c r="K114" s="41" t="s">
-        <v>304</v>
+        <v>237</v>
       </c>
     </row>
     <row r="115" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B115" s="3" t="s">
-        <v>71</v>
+      <c r="B115" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>240</v>
+        <v>301</v>
       </c>
       <c r="D115" s="6">
         <v>1</v>
       </c>
       <c r="E115" s="7">
-        <v>12000</v>
-      </c>
-      <c r="F115" s="8" t="s">
-        <v>13</v>
+        <v>17900</v>
+      </c>
+      <c r="F115" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="G115" s="7">
         <f t="shared" si="0"/>
-        <v>12000</v>
+        <v>17900</v>
       </c>
       <c r="H115" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I115" s="10" t="s">
-        <v>241</v>
+        <v>76</v>
       </c>
       <c r="J115" s="10" t="s">
-        <v>241</v>
+        <v>76</v>
       </c>
       <c r="K115" s="41" t="s">
-        <v>240</v>
+        <v>301</v>
       </c>
     </row>
     <row r="116" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B116" s="33" t="s">
+      <c r="B116" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D116" s="11">
+        <v>240</v>
+      </c>
+      <c r="D116" s="6">
         <v>1</v>
       </c>
       <c r="E116" s="7">
-        <v>11000</v>
-      </c>
-      <c r="F116" s="27" t="s">
+        <v>13000</v>
+      </c>
+      <c r="F116" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G116" s="7">
         <f t="shared" si="0"/>
-        <v>11000</v>
+        <v>13000</v>
       </c>
       <c r="H116" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I116" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="J116" s="16" t="s">
-        <v>243</v>
+      <c r="I116" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="J116" s="10" t="s">
+        <v>241</v>
       </c>
       <c r="K116" s="41" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="33" t="s">
         <v>71</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D117" s="6">
+        <v>242</v>
+      </c>
+      <c r="D117" s="11">
         <v>1</v>
       </c>
       <c r="E117" s="7">
         <v>12000</v>
       </c>
-      <c r="F117" s="8" t="s">
+      <c r="F117" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G117" s="7">
@@ -5936,14 +6012,14 @@
       <c r="H117" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I117" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J117" s="10" t="s">
-        <v>16</v>
+      <c r="I117" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="J117" s="16" t="s">
+        <v>243</v>
       </c>
       <c r="K117" s="41" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="118" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5954,68 +6030,68 @@
         <v>71</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D118" s="6">
         <v>1</v>
       </c>
       <c r="E118" s="7">
-        <v>15000</v>
-      </c>
-      <c r="F118" s="28" t="s">
-        <v>211</v>
+        <v>12000</v>
+      </c>
+      <c r="F118" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="G118" s="7">
         <f t="shared" si="0"/>
-        <v>15000</v>
+        <v>12000</v>
       </c>
       <c r="H118" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I118" s="10" t="s">
-        <v>246</v>
+        <v>16</v>
       </c>
       <c r="J118" s="10" t="s">
-        <v>247</v>
+        <v>16</v>
       </c>
       <c r="K118" s="41" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="119" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B119" s="22" t="s">
-        <v>137</v>
+      <c r="B119" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D119" s="6">
         <v>1</v>
       </c>
       <c r="E119" s="7">
-        <v>8000</v>
-      </c>
-      <c r="F119" s="8" t="s">
-        <v>13</v>
+        <v>15000</v>
+      </c>
+      <c r="F119" s="28" t="s">
+        <v>211</v>
       </c>
       <c r="G119" s="7">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>15000</v>
       </c>
       <c r="H119" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I119" s="10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="J119" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K119" s="41" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6026,32 +6102,32 @@
         <v>137</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D120" s="6">
         <v>1</v>
       </c>
       <c r="E120" s="7">
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="F120" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G120" s="7">
-        <f t="shared" ref="G120" si="8">D120*E120</f>
-        <v>8000</v>
+        <f t="shared" si="0"/>
+        <v>10000</v>
       </c>
       <c r="H120" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I120" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J120" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K120" s="41" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="121" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6062,20 +6138,20 @@
         <v>137</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>287</v>
+        <v>250</v>
       </c>
       <c r="D121" s="6">
         <v>1</v>
       </c>
       <c r="E121" s="7">
-        <v>8500</v>
+        <v>10000</v>
       </c>
       <c r="F121" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G121" s="7">
-        <f>D121*E121</f>
-        <v>8500</v>
+        <f t="shared" ref="G121" si="9">D121*E121</f>
+        <v>10000</v>
       </c>
       <c r="H121" s="13" t="s">
         <v>183</v>
@@ -6087,7 +6163,7 @@
         <v>251</v>
       </c>
       <c r="K121" s="41" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
     </row>
     <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6098,32 +6174,32 @@
         <v>137</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>318</v>
+        <v>287</v>
       </c>
       <c r="D122" s="6">
         <v>1</v>
       </c>
       <c r="E122" s="7">
-        <v>9000</v>
+        <v>8500</v>
       </c>
       <c r="F122" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G122" s="7">
         <f>D122*E122</f>
-        <v>9000</v>
+        <v>8500</v>
       </c>
       <c r="H122" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I122" s="10" t="s">
-        <v>319</v>
+        <v>251</v>
       </c>
       <c r="J122" s="10" t="s">
-        <v>319</v>
+        <v>251</v>
       </c>
       <c r="K122" s="41" t="s">
-        <v>318</v>
+        <v>286</v>
       </c>
     </row>
     <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6134,29 +6210,32 @@
         <v>137</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>252</v>
+        <v>314</v>
       </c>
       <c r="D123" s="6">
         <v>1</v>
       </c>
       <c r="E123" s="7">
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="F123" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G123" s="7">
-        <f t="shared" si="0"/>
-        <v>7000</v>
+        <f>D123*E123</f>
+        <v>10000</v>
       </c>
       <c r="H123" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I123" s="10" t="s">
-        <v>253</v>
+        <v>315</v>
       </c>
       <c r="J123" s="10" t="s">
-        <v>253</v>
+        <v>315</v>
+      </c>
+      <c r="K123" s="41" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="124" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6167,32 +6246,29 @@
         <v>137</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D124" s="6">
         <v>1</v>
       </c>
       <c r="E124" s="7">
-        <v>14000</v>
-      </c>
-      <c r="F124" s="28" t="s">
-        <v>211</v>
+        <v>12000</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="G124" s="7">
         <f t="shared" si="0"/>
-        <v>14000</v>
+        <v>12000</v>
       </c>
       <c r="H124" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I124" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J124" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="K124" s="41" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="125" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6203,32 +6279,32 @@
         <v>137</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D125" s="6">
         <v>1</v>
       </c>
       <c r="E125" s="7">
-        <v>7000</v>
-      </c>
-      <c r="F125" s="12" t="s">
-        <v>33</v>
+        <v>16000</v>
+      </c>
+      <c r="F125" s="28" t="s">
+        <v>211</v>
       </c>
       <c r="G125" s="7">
         <f t="shared" si="0"/>
-        <v>7000</v>
+        <v>16000</v>
       </c>
       <c r="H125" s="13" t="s">
         <v>183</v>
       </c>
       <c r="I125" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J125" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="K125" s="50" t="s">
-        <v>256</v>
+        <v>255</v>
+      </c>
+      <c r="K125" s="41" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6239,20 +6315,20 @@
         <v>137</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>303</v>
+        <v>256</v>
       </c>
       <c r="D126" s="6">
         <v>1</v>
       </c>
       <c r="E126" s="7">
-        <v>9900</v>
+        <v>8000</v>
       </c>
       <c r="F126" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G126" s="7">
-        <f t="shared" ref="G126:G127" si="9">D126*E126</f>
-        <v>9900</v>
+        <f t="shared" si="0"/>
+        <v>8000</v>
       </c>
       <c r="H126" s="13" t="s">
         <v>183</v>
@@ -6264,320 +6340,355 @@
         <v>257</v>
       </c>
       <c r="K126" s="50" t="s">
-        <v>303</v>
+        <v>256</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B127" s="47" t="s">
-        <v>292</v>
-      </c>
-      <c r="C127" s="48" t="s">
-        <v>293</v>
+      <c r="B127" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="D127" s="6">
         <v>1</v>
       </c>
       <c r="E127" s="7">
-        <v>52000</v>
+        <v>11000</v>
       </c>
       <c r="F127" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G127" s="7">
-        <f t="shared" si="9"/>
-        <v>52000</v>
+        <f t="shared" ref="G127:G128" si="10">D127*E127</f>
+        <v>11000</v>
       </c>
       <c r="H127" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I127" s="49" t="s">
-        <v>294</v>
-      </c>
-      <c r="J127" s="49" t="s">
-        <v>295</v>
+      <c r="I127" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="J127" s="10" t="s">
+        <v>257</v>
       </c>
       <c r="K127" s="50" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
     </row>
     <row r="128" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B128" s="43" t="s">
-        <v>269</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>270</v>
+      <c r="B128" s="47" t="s">
+        <v>291</v>
+      </c>
+      <c r="C128" s="48" t="s">
+        <v>292</v>
       </c>
       <c r="D128" s="6">
         <v>1</v>
       </c>
       <c r="E128" s="7">
-        <v>16000</v>
+        <v>52000</v>
       </c>
       <c r="F128" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G128" s="7">
-        <f t="shared" si="0"/>
-        <v>16000</v>
+        <f t="shared" si="10"/>
+        <v>52000</v>
       </c>
       <c r="H128" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I128" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="J128" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="K128" s="41" t="s">
-        <v>270</v>
+      <c r="I128" s="49" t="s">
+        <v>293</v>
+      </c>
+      <c r="J128" s="49" t="s">
+        <v>294</v>
+      </c>
+      <c r="K128" s="50" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="129" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B129" s="34" t="s">
-        <v>258</v>
+      <c r="B129" s="43" t="s">
+        <v>269</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="D129" s="6">
         <v>1</v>
       </c>
       <c r="E129" s="7">
+        <v>16000</v>
+      </c>
+      <c r="F129" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G129" s="7">
+        <f t="shared" si="0"/>
+        <v>16000</v>
+      </c>
+      <c r="H129" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="I129" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="J129" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="K129" s="41" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B130" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D130" s="6">
+        <v>1</v>
+      </c>
+      <c r="E130" s="7">
         <v>17000</v>
       </c>
-      <c r="F129" s="28" t="s">
+      <c r="F130" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="G129" s="7">
-        <f t="shared" ref="G129" si="10">D129*E129</f>
+      <c r="G130" s="7">
+        <f t="shared" ref="G130" si="11">D130*E130</f>
         <v>17000</v>
       </c>
-      <c r="H129" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="I129" s="10" t="s">
+      <c r="H130" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="I130" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="J129" s="10" t="s">
+      <c r="J130" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="K129" s="41" t="s">
+      <c r="K130" s="41" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
+    <row r="131" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="B131" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="C131" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="D131" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E130" s="3" t="s">
+      <c r="E131" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="F130" s="3" t="s">
+      <c r="F131" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G130" s="3" t="s">
+      <c r="G131" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H130" s="3" t="s">
+      <c r="H131" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="I130" s="3" t="s">
+      <c r="I131" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="J130" s="3" t="s">
+      <c r="J131" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="4" t="str">
-        <f>"En curso = " &amp; COUNTA(A2:A30)</f>
-        <v>En curso = 29</v>
-      </c>
-      <c r="B131" s="14" t="str">
-        <f>"Ivrea = " &amp; COUNTA(B13:B25,B35:B51,B63:B111)</f>
-        <v>Ivrea = 79</v>
-      </c>
-      <c r="C131" s="45" t="str">
-        <f>"Series en total = " &amp; COUNTA(C2:C129)</f>
-        <v>Series en total = 128</v>
-      </c>
-      <c r="D131" s="6">
-        <f>SUM(D2:D129)</f>
-        <v>576</v>
-      </c>
-      <c r="E131" s="7">
-        <f>SUM(E2:E129)</f>
-        <v>1447466</v>
-      </c>
-      <c r="F131" s="46" t="str">
-        <f>"B6 = " &amp; COUNTA(F2:F11,F13:F14,F26,F31:F34,F39:F52,F56:F58,F60:F62,F70:F89,F112,F115:F117,F119:F123)</f>
-        <v>B6 = 66</v>
-      </c>
-      <c r="G131" s="7">
-        <f>SUM(G2:G129)</f>
-        <v>5792498</v>
-      </c>
-      <c r="H131" s="13" t="str">
-        <f>"Finalizados = " &amp; COUNTA(H7,H27:H29,H31:H59,H61:H64,H70,H72:H129)</f>
+    <row r="132" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="str">
+        <f>"En curso = " &amp; COUNTA(A2:A29)</f>
+        <v>En curso = 28</v>
+      </c>
+      <c r="B132" s="14" t="str">
+        <f>"Ivrea = " &amp; COUNTA(B12:B25,B35:B51,B64:B112)</f>
+        <v>Ivrea = 80</v>
+      </c>
+      <c r="C132" s="45" t="str">
+        <f>"Series en total = " &amp; COUNTA(C2:C130)</f>
+        <v>Series en total = 129</v>
+      </c>
+      <c r="D132" s="6">
+        <f>SUM(D2:D130)</f>
+        <v>585</v>
+      </c>
+      <c r="E132" s="7">
+        <f>SUM(E2:E130)</f>
+        <v>1542900</v>
+      </c>
+      <c r="F132" s="46" t="str">
+        <f>"B6 = " &amp; COUNTA(F2:F10,F12:F14,F26,F30:F34,F39:F52,F57:F59,F61:F63,F71:F90,F113,F116:F118,F120:F124)</f>
+        <v>B6 = 67</v>
+      </c>
+      <c r="G132" s="7">
+        <f>SUM(G2:G130)</f>
+        <v>6266600</v>
+      </c>
+      <c r="H132" s="13" t="str">
+        <f>"Finalizados = " &amp; COUNTA(H27:H28,H30:H60,H62:H65,H71,H73:H130)</f>
         <v>Finalizados = 96</v>
       </c>
-      <c r="I131" s="46" t="str">
-        <f>"B6 = " &amp; SUM(D2:D11,D13:D14,D26,D31:D34,D39:D52,D56:D58,D60:D62,D70:D89,D112,D115:D117,D119:D123)</f>
-        <v>B6 = 306</v>
-      </c>
-      <c r="J131" s="35" t="str">
-        <f>"Series = " &amp; COUNTA(K2:K6,K8:K17,K19:K24,K26:K31,K33:K34,K37:K43,K52:K57,K59,K72,K82:K92,K94,K100:K101,K103,K105:K109,K113:K122,K124:K129)</f>
-        <v>Series = 80</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="20" t="str">
-        <f>"Completado = " &amp; COUNTA(A31:A59)</f>
-        <v>Completado = 29</v>
-      </c>
-      <c r="B132" s="5" t="str">
-        <f>"Panini = " &amp; COUNTA(B2:B12,B31:B34,B60:B62)</f>
+      <c r="I132" s="46" t="str">
+        <f>"B6 = " &amp; SUM(D2:D10,D12:D14,D26,D30:D34,D39:D52,D57:D59,D61:D63,D71:D90,D113,D116:D118,D120:D124)</f>
+        <v>B6 = 311</v>
+      </c>
+      <c r="J132" s="35" t="str">
+        <f>"Series = " &amp; COUNTA(K2:K6,K7:K17,K19:K24,K26:K30,K33:K34,K37:K43,K52:K58,K60,K73,K83:K93,K95,K101:K102,K104,K106:K110,K114:K123,K125:K130)</f>
+        <v>Series = 81</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="20" t="str">
+        <f>"Completado = " &amp; COUNTA(A30:A60)</f>
+        <v>Completado = 31</v>
+      </c>
+      <c r="B133" s="5" t="str">
+        <f>"Panini = " &amp; COUNTA(B2:B11,B30:B34,B61:B63)</f>
         <v>Panini = 18</v>
       </c>
-      <c r="F132" s="39" t="str">
-        <f>"C6 = " &amp; COUNTA(F15:F23,F35:F38,F59,F63:F69,F95:F104)</f>
+      <c r="F133" s="39" t="str">
+        <f>"C6 = " &amp; COUNTA(F15:F23,F35:F38,F60,F64:F70,F96:F105)</f>
         <v>C6 = 31</v>
       </c>
-      <c r="H132" s="9" t="str">
-        <f>"En publicación = " &amp; COUNTA(H2:H6,H8:H26,H30,H60,H65:H69,H71)</f>
-        <v>En publicación = 32</v>
-      </c>
-      <c r="I132" s="39" t="str">
-        <f>"C6 = " &amp; SUM(D15:D23,D35:D38,D59,D63:D69,D95:D104)</f>
-        <v>C6 = 207</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="25" t="str">
-        <f>"Droppeado = " &amp; COUNTA(A60:A71)</f>
+      <c r="H133" s="9" t="str">
+        <f>"En publicación = " &amp; COUNTA(H2:H26,H29,H61,H66:H70,H72)</f>
+        <v>En publicación = 33</v>
+      </c>
+      <c r="I133" s="39" t="str">
+        <f>"C6 = " &amp; SUM(D15:D23,D35:D38,D60,D64:D70,D96:D105)</f>
+        <v>C6 = 210</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="25" t="str">
+        <f>"Droppeado = " &amp; COUNTA(A61:A72)</f>
         <v>Droppeado = 12</v>
       </c>
-      <c r="B133" s="22" t="str">
-        <f>"Kemuri = " &amp; COUNTA(B55,B119:B126)</f>
+      <c r="B134" s="22" t="str">
+        <f>"Kemuri = " &amp; COUNTA(B56,B120:B127)</f>
         <v>Kemuri = 9</v>
       </c>
-      <c r="F133" s="40" t="str">
-        <f>"A5 = " &amp; COUNTA(F12,F25,F27:F29,F53:F55,F107:F110,F113:F114,F125:F128)</f>
-        <v>A5 = 18</v>
-      </c>
-      <c r="I133" s="40" t="str">
-        <f>"A5 = " &amp; SUM(D12,D25,D27:D29,D53:D55,D107:D110,D113:D114,D125:D128)</f>
-        <v>A5 = 41</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="26" t="str">
-        <f>"Tomo único = " &amp; COUNTA(A72:A129)</f>
+      <c r="F134" s="40" t="str">
+        <f>"A5 = " &amp; COUNTA(F11,F25,F27:F55,F53:F56,F108:F111,F114:F115,F126:F129)</f>
+        <v>A5 = 45</v>
+      </c>
+      <c r="I134" s="40" t="str">
+        <f>"A5 = " &amp; SUM(D11,D25,D27:D55,D53:D56,D108:D111,D114:D115,D126:D129)</f>
+        <v>A5 = 260</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="26" t="str">
+        <f>"Tomo único = " &amp; COUNTA(A73:A130)</f>
         <v>Tomo único = 58</v>
       </c>
-      <c r="B134" s="23" t="str">
-        <f>"Distrito Manga = " &amp; COUNTA(B56:B57,B114)</f>
+      <c r="B135" s="23" t="str">
+        <f>"Distrito Manga = " &amp; COUNTA(B57:B58,B115)</f>
         <v>Distrito Manga = 3</v>
       </c>
-      <c r="F134" s="28" t="str">
-        <f>"B6x2 = " &amp; COUNTA(F90:F94,F118,F124,F129:F129)</f>
+      <c r="F135" s="28" t="str">
+        <f>"B6x2 = " &amp; COUNTA(F91:F95,F119,F125,F130:F130)</f>
         <v>B6x2 = 8</v>
       </c>
-      <c r="I134" s="28" t="str">
-        <f>"B6x2 = " &amp; SUM(D90:D94,D118,D124,D129:D129)</f>
+      <c r="I135" s="28" t="str">
+        <f>"B6x2 = " &amp; SUM(D91:D95,D119,D125,D130:D130)</f>
         <v>B6x2 = 8</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="3" t="str">
-        <f>"Ovni Press = " &amp; COUNTA(B26,B115:B118)</f>
+    <row r="136" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="3" t="str">
+        <f>"Ovni Press = " &amp; COUNTA(B26,B116:B119)</f>
         <v>Ovni Press = 5</v>
       </c>
-      <c r="F135" s="30" t="str">
-        <f>"C6x2 = " &amp; COUNTA(F105:F106)</f>
+      <c r="F136" s="30" t="str">
+        <f>"C6x2 = " &amp; COUNTA(F106:F107)</f>
         <v>C6x2 = 2</v>
       </c>
-      <c r="I135" s="30" t="str">
-        <f>"C6x2 = " &amp; SUM(D105:D106)</f>
+      <c r="I136" s="30" t="str">
+        <f>"C6x2 = " &amp; SUM(D106:D107)</f>
         <v>C6x2 = 2</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="36" t="str">
-        <f>"Planeta Cómic = " &amp; COUNTA(B27:B28,B52:B53,B114)</f>
+    <row r="137" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="36" t="str">
+        <f>"Planeta Cómic = " &amp; COUNTA(B27:B28,B52:B53,B115)</f>
         <v>Planeta Cómic = 5</v>
       </c>
-      <c r="F136" s="17" t="str">
-        <f>"A5 color = " &amp; COUNTA(F24,F30,F111)</f>
+      <c r="F137" s="17" t="str">
+        <f>"A5 color = " &amp; COUNTA(F24,F29,F112)</f>
         <v>A5 color = 3</v>
       </c>
-      <c r="I136" s="17" t="str">
-        <f>"A5 color = " &amp; SUM(D111,D24,D30)</f>
-        <v>A5 color = 12</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="24" t="str">
-        <f>"Utopia = " &amp; COUNTA(B58:B59)</f>
+      <c r="I137" s="17" t="str">
+        <f>"A5 color = " &amp; SUM(D112,D24,D29)</f>
+        <v>A5 color = 13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="24" t="str">
+        <f>"Utopia = " &amp; COUNTA(B59:B60)</f>
         <v>Utopia = 2</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="21" t="str">
+    <row r="139" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="21" t="str">
         <f>"Merci = " &amp; COUNTA(B54)</f>
         <v>Merci = 1</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="32" t="str">
-        <f>"Milky Way = " &amp; COUNTA(B112)</f>
+    <row r="140" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="32" t="str">
+        <f>"Milky Way = " &amp; COUNTA(B113)</f>
         <v>Milky Way = 1</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="37" t="str">
-        <f>"Moztros = " &amp; COUNTA(B29,B129)</f>
+    <row r="141" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="37" t="str">
+        <f>"Moztros = " &amp; COUNTA(B55,B130)</f>
         <v>Moztros = 2</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="38" t="str">
-        <f>"Random Comics = " &amp; COUNTA(B30)</f>
+    <row r="142" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="38" t="str">
+        <f>"Random Comics = " &amp; COUNTA(B29)</f>
         <v>Random Comics = 1</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="43" t="str">
-        <f>"Hotel de las Ideas = " &amp; COUNTA(B128)</f>
+    <row r="143" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="43" t="str">
+        <f>"Hotel de las Ideas = " &amp; COUNTA(B129)</f>
         <v>Hotel de las Ideas = 1</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="47" t="str">
-        <f>"Kibook Ediciones = " &amp; COUNTA(B127)</f>
+    <row r="144" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="47" t="str">
+        <f>"Kibook Ediciones = " &amp; COUNTA(B128)</f>
         <v>Kibook Ediciones = 1</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7435,79 +7546,109 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="F2:F9 F11:F120 F122:F130">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+  <conditionalFormatting sqref="F123:F131 F10:F12 F2:F8 F14:F121">
+    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
       <formula>"B6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3 F8:F9 F11:F33 F35:F120 F122:F130">
-    <cfRule type="cellIs" dxfId="15" priority="37" operator="equal">
+  <conditionalFormatting sqref="F3 F7:F8 F123:F131 F10:F12 F14:F33 F35:F121">
+    <cfRule type="cellIs" dxfId="23" priority="45" operator="equal">
       <formula>"C6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="46" operator="equal">
       <formula>"A5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14 F39">
-    <cfRule type="cellIs" dxfId="13" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="49" operator="equal">
       <formula>"B6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="50" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="51" operator="equal">
       <formula>"C6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="52" operator="equal">
       <formula>"A5"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H7 H61:H64 H70 H27:H29 H31:H59 H72:H120 H122:H130">
-    <cfRule type="containsText" dxfId="9" priority="39" operator="containsText" text="En publicacion">
+  <conditionalFormatting sqref="H62:H65 H71 H73:H121 H123:H131 H4:H6 H27:H28 H30:H60">
+    <cfRule type="containsText" dxfId="17" priority="47" operator="containsText" text="En publicacion">
       <formula>NOT(ISERROR(SEARCH(("En publicacion"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+  <conditionalFormatting sqref="F9">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"B6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+  <conditionalFormatting sqref="F9">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"C6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"A5"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F121">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+  <conditionalFormatting sqref="F122">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"B6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F121">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="F122">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"C6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"A5"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H121">
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="En publicacion">
-      <formula>NOT(ISERROR(SEARCH(("En publicacion"),(H121))))</formula>
+  <conditionalFormatting sqref="H122">
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="En publicacion">
+      <formula>NOT(ISERROR(SEARCH(("En publicacion"),(H122))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"B6"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"C6"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"A5"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"B6"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+      <formula>"C6"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+      <formula>"A5"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>